<commit_message>
Primeiro upload, ainda com arquivos antigos
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -406,6 +406,12 @@
   <si>
     <t xml:space="preserve">ccih@hpa.org</t>
   </si>
+  <si>
+    <t xml:space="preserve">taline@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hlanziotti@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -72925,6 +72931,4820 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2490">
+      <c r="A2490" s="1" t="n">
+        <v>43997.1091483912</v>
+      </c>
+      <c r="B2490" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2490" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2490" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2490" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2490" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2490" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2490" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2490" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2491">
+      <c r="A2491" s="1" t="n">
+        <v>43997.3248068981</v>
+      </c>
+      <c r="B2491" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2491" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2491" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2491" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2491" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2491" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2491" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2491" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2492">
+      <c r="A2492" s="1" t="n">
+        <v>43997.3330781829</v>
+      </c>
+      <c r="B2492" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2492" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2492" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2492" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2492" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2492" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2492" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2492" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2493">
+      <c r="A2493" s="1" t="n">
+        <v>43997.3333521644</v>
+      </c>
+      <c r="B2493" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2493" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2493" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2493" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2493" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2493" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2493" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2493" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2494">
+      <c r="A2494" s="1" t="n">
+        <v>43997.3563485532</v>
+      </c>
+      <c r="B2494" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2494" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2494" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2494" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2494" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2494" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2494" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2494" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2495">
+      <c r="A2495" s="1" t="n">
+        <v>43997.3595324306</v>
+      </c>
+      <c r="B2495" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2495" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2495" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2495" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2495" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2495" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2495" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2495" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2496">
+      <c r="A2496" s="1" t="n">
+        <v>43997.3682553935</v>
+      </c>
+      <c r="B2496" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2496" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2496" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2496" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2496" t="n">
+        <v>61</v>
+      </c>
+      <c r="G2496" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2496" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2496" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2497">
+      <c r="A2497" s="1" t="n">
+        <v>43997.3692383681</v>
+      </c>
+      <c r="B2497" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2497" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2497" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2497" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2497" t="n">
+        <v>63</v>
+      </c>
+      <c r="G2497" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2497" t="n">
+        <v>19</v>
+      </c>
+      <c r="I2497" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2498">
+      <c r="A2498" s="1" t="n">
+        <v>43997.3749967593</v>
+      </c>
+      <c r="B2498" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2498" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2498" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2498" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2498" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2498" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2498" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2498" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2499">
+      <c r="A2499" s="1" t="n">
+        <v>43997.3853217593</v>
+      </c>
+      <c r="B2499" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2499" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2499" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2499" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2499" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2499" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2499" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2499" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2500">
+      <c r="A2500" s="1" t="n">
+        <v>43997.4033918866</v>
+      </c>
+      <c r="B2500" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2500" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2500" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2500" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2500" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2500" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2500" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2500" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2501">
+      <c r="A2501" s="1" t="n">
+        <v>43997.4034255324</v>
+      </c>
+      <c r="B2501" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2501" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2501" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2501" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2501" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2501" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2501" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2501" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2502">
+      <c r="A2502" s="1" t="n">
+        <v>43997.4034607523</v>
+      </c>
+      <c r="B2502" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2502" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2502" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2502" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2502" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2502" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2502" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2502" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2503">
+      <c r="A2503" s="1" t="n">
+        <v>43997.4043494676</v>
+      </c>
+      <c r="B2503" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2503" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2503" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2503" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2503" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2503" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2503" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2503" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2504">
+      <c r="A2504" s="1" t="n">
+        <v>43997.4064716551</v>
+      </c>
+      <c r="B2504" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2504" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2504" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2504" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2504" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2504" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2504" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2504" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2505">
+      <c r="A2505" s="1" t="n">
+        <v>43997.422886412</v>
+      </c>
+      <c r="B2505" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2505" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2505" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2505" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2505" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2505" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2505" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2505" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2506">
+      <c r="A2506" s="1" t="n">
+        <v>43997.4245183102</v>
+      </c>
+      <c r="B2506" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2506" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2506" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2506" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2506" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2506" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2506" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2506" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2507">
+      <c r="A2507" s="1" t="n">
+        <v>43997.4385315046</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2507" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2507" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2507" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2507" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2507" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2507" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2507" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2508">
+      <c r="A2508" s="1" t="n">
+        <v>43997.4614446296</v>
+      </c>
+      <c r="B2508" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2508" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2508" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2508" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2508" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2508" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2508" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2508" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2509">
+      <c r="A2509" s="1" t="n">
+        <v>43997.4642227199</v>
+      </c>
+      <c r="B2509" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2509" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2509" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2509" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2509" t="n">
+        <v>68</v>
+      </c>
+      <c r="G2509" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2509" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2509" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2510">
+      <c r="A2510" s="1" t="n">
+        <v>43997.4654589583</v>
+      </c>
+      <c r="B2510" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2510" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2510" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2510" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2510" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2510" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2510" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2510" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2511">
+      <c r="A2511" s="1" t="n">
+        <v>43997.4659311458</v>
+      </c>
+      <c r="B2511" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2511" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2511" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2511" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2511" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2511" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2511" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2511" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2512">
+      <c r="A2512" s="1" t="n">
+        <v>43997.4770096065</v>
+      </c>
+      <c r="B2512" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2512" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2512" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2512" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2512" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2512" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2512" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2512" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2513">
+      <c r="A2513" s="1" t="n">
+        <v>43997.4849310995</v>
+      </c>
+      <c r="B2513" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2513" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2513" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2513" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2513" t="n">
+        <v>81</v>
+      </c>
+      <c r="G2513" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2513" t="n">
+        <v>30</v>
+      </c>
+      <c r="I2513" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2514">
+      <c r="A2514" s="1" t="n">
+        <v>43997.4853847454</v>
+      </c>
+      <c r="B2514" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2514" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2514" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2514" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2514" t="n">
+        <v>85</v>
+      </c>
+      <c r="G2514" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2514" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2514" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2515">
+      <c r="A2515" s="1" t="n">
+        <v>43997.4862898264</v>
+      </c>
+      <c r="B2515" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2515" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2515" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2515" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2515" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2515" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2515" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2515" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2516">
+      <c r="A2516" s="1" t="n">
+        <v>43997.5215275116</v>
+      </c>
+      <c r="B2516" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2516" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2516" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2516" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2516" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2516" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2516" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2516" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2517">
+      <c r="A2517" s="1" t="n">
+        <v>43997.5330368287</v>
+      </c>
+      <c r="B2517" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2517" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2517" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2517" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2517" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2517" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2517" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2517" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2518">
+      <c r="A2518" s="1" t="n">
+        <v>43997.5575211921</v>
+      </c>
+      <c r="B2518" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2518" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2518" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2518" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2518" t="n">
+        <v>63</v>
+      </c>
+      <c r="G2518" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2518" t="n">
+        <v>19</v>
+      </c>
+      <c r="I2518" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2519">
+      <c r="A2519" s="1" t="n">
+        <v>43997.565912338</v>
+      </c>
+      <c r="B2519" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2519" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2519" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2519" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2519" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2519" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2519" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2519" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2520">
+      <c r="A2520" s="1" t="n">
+        <v>43997.5683260648</v>
+      </c>
+      <c r="B2520" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2520" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2520" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2520" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2520" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2520" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2520" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2520" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2521">
+      <c r="A2521" s="1" t="n">
+        <v>43997.5734814352</v>
+      </c>
+      <c r="B2521" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2521" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2521" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2521" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2521" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2521" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2521" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2521" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2522">
+      <c r="A2522" s="1" t="n">
+        <v>43997.6133413426</v>
+      </c>
+      <c r="B2522" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2522" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2522" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2522" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2522" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2522" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2522" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2522" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2523">
+      <c r="A2523" s="1" t="n">
+        <v>43997.6238787269</v>
+      </c>
+      <c r="B2523" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2523" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2523" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2523" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2523" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2523" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2523" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2523" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2524">
+      <c r="A2524" s="1" t="n">
+        <v>43997.6788384722</v>
+      </c>
+      <c r="B2524" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2524" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2524" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2524" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2524" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2524" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2524" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2524" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2525">
+      <c r="A2525" s="1" t="n">
+        <v>43997.6943168403</v>
+      </c>
+      <c r="B2525" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2525" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2525" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2525" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2525" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2525" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2525" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2525" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2526">
+      <c r="A2526" s="1" t="n">
+        <v>43997.7309387268</v>
+      </c>
+      <c r="B2526" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2526" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2526" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2526" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2526" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2526" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2526" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2526" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2527">
+      <c r="A2527" s="1" t="n">
+        <v>43997.7536562153</v>
+      </c>
+      <c r="B2527" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2527" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2527" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2527" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2527" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2527" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2527" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2527" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2528">
+      <c r="A2528" s="1" t="n">
+        <v>43997.7849013079</v>
+      </c>
+      <c r="B2528" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2528" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2528" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2528" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2528" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2528" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2528" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2528" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2529">
+      <c r="A2529" s="1" t="n">
+        <v>43997.8826364583</v>
+      </c>
+      <c r="B2529" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2529" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2529" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2529" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2529" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2529" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2529" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2529" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2530">
+      <c r="A2530" s="1" t="n">
+        <v>43998.1340864468</v>
+      </c>
+      <c r="B2530" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2530" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2530" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2530" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2530" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2530" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2530" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2530" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2531">
+      <c r="A2531" s="1" t="n">
+        <v>43998.3137349421</v>
+      </c>
+      <c r="B2531" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2531" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2531" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2531" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2531" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2531" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2531" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2531" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2532">
+      <c r="A2532" s="1" t="n">
+        <v>43998.3155470949</v>
+      </c>
+      <c r="B2532" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2532" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2532" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2532" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2532" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2532" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2532" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2532" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2533">
+      <c r="A2533" s="1" t="n">
+        <v>43998.3243499537</v>
+      </c>
+      <c r="B2533" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2533" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2533" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2533" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2533" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2533" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2533" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2533" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2534">
+      <c r="A2534" s="1" t="n">
+        <v>43998.3547959028</v>
+      </c>
+      <c r="B2534" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2534" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2534" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2534" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2534" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2534" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2534" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2534" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2535">
+      <c r="A2535" s="1" t="n">
+        <v>43998.3633885185</v>
+      </c>
+      <c r="B2535" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2535" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2535" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2535" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2535" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2535" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2535" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2535" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2536">
+      <c r="A2536" s="1" t="n">
+        <v>43998.3729975694</v>
+      </c>
+      <c r="B2536" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2536" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2536" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2536" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2536" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2536" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2536" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2536" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2537">
+      <c r="A2537" s="1" t="n">
+        <v>43998.3745767014</v>
+      </c>
+      <c r="B2537" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2537" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2537" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2537" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2537" t="n">
+        <v>85</v>
+      </c>
+      <c r="G2537" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2537" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2537" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2538">
+      <c r="A2538" s="1" t="n">
+        <v>43998.375634537</v>
+      </c>
+      <c r="B2538" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2538" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2538" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2538" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2538" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2538" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2538" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2538" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2539">
+      <c r="A2539" s="1" t="n">
+        <v>43998.3869337963</v>
+      </c>
+      <c r="B2539" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2539" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2539" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2539" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2539" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2539" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2539" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2539" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2540">
+      <c r="A2540" s="1" t="n">
+        <v>43998.3901838079</v>
+      </c>
+      <c r="B2540" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2540" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2540" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2540" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2540" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2540" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2540" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2540" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2541">
+      <c r="A2541" s="1" t="n">
+        <v>43998.3914920139</v>
+      </c>
+      <c r="B2541" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2541" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2541" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2541" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2541" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2541" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2541" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2541" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2542">
+      <c r="A2542" s="1" t="n">
+        <v>43998.3966894213</v>
+      </c>
+      <c r="B2542" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2542" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2542" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2542" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2542" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2542" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2542" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2542" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2543">
+      <c r="A2543" s="1" t="n">
+        <v>43998.403306088</v>
+      </c>
+      <c r="B2543" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2543" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2543" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2543" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2543" t="n">
+        <v>47</v>
+      </c>
+      <c r="G2543" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2543" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2543" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2544">
+      <c r="A2544" s="1" t="n">
+        <v>43998.412968588</v>
+      </c>
+      <c r="B2544" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2544" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2544" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2544" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2544" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2544" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2544" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2544" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2545">
+      <c r="A2545" s="1" t="n">
+        <v>43998.4466110185</v>
+      </c>
+      <c r="B2545" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2545" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2545" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2545" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2545" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2545" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2545" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2545" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2546">
+      <c r="A2546" s="1" t="n">
+        <v>43998.4486882523</v>
+      </c>
+      <c r="B2546" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2546" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2546" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2546" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2546" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2546" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2546" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2546" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2547">
+      <c r="A2547" s="1" t="n">
+        <v>43998.4584168056</v>
+      </c>
+      <c r="B2547" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2547" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2547" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2547" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2547" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2547" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2547" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2547" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2548">
+      <c r="A2548" s="1" t="n">
+        <v>43998.4661150579</v>
+      </c>
+      <c r="B2548" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2548" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2548" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2548" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2548" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2548" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2548" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2548" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2549">
+      <c r="A2549" s="1" t="n">
+        <v>43998.4665067014</v>
+      </c>
+      <c r="B2549" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2549" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2549" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2549" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2549" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2549" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2549" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2549" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2550">
+      <c r="A2550" s="1" t="n">
+        <v>43998.4674939352</v>
+      </c>
+      <c r="B2550" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2550" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2550" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2550" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2550" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2550" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2550" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2550" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2551">
+      <c r="A2551" s="1" t="n">
+        <v>43998.4676078935</v>
+      </c>
+      <c r="B2551" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2551" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2551" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2551" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2551" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2551" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2551" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2551" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2552">
+      <c r="A2552" s="1" t="n">
+        <v>43998.468946713</v>
+      </c>
+      <c r="B2552" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2552" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2552" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2552" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2552" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2552" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2552" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2552" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2553">
+      <c r="A2553" s="1" t="n">
+        <v>43998.4690828819</v>
+      </c>
+      <c r="B2553" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2553" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2553" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2553" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2553" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2553" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2553" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2553" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2554">
+      <c r="A2554" s="1" t="n">
+        <v>43998.4692215162</v>
+      </c>
+      <c r="B2554" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2554" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2554" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2554" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2554" t="n">
+        <v>69</v>
+      </c>
+      <c r="G2554" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2554" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2554" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2555">
+      <c r="A2555" s="1" t="n">
+        <v>43998.470486412</v>
+      </c>
+      <c r="B2555" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2555" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2555" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2555" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2555" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2555" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2555" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2555" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2556">
+      <c r="A2556" s="1" t="n">
+        <v>43998.495690544</v>
+      </c>
+      <c r="B2556" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2556" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2556" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2556" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2556" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2556" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2556" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2556" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2557">
+      <c r="A2557" s="1" t="n">
+        <v>43998.4995803704</v>
+      </c>
+      <c r="B2557" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2557" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2557" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2557" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2557" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2557" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2557" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2557" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2558">
+      <c r="A2558" s="1" t="n">
+        <v>43998.5102359143</v>
+      </c>
+      <c r="B2558" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2558" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2558" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2558" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2558" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2558" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2558" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2558" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2559">
+      <c r="A2559" s="1" t="n">
+        <v>43998.5107386111</v>
+      </c>
+      <c r="B2559" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2559" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2559" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2559" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2559" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2559" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2559" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2559" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2560">
+      <c r="A2560" s="1" t="n">
+        <v>43998.5168312847</v>
+      </c>
+      <c r="B2560" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2560" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2560" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2560" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2560" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2560" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2560" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2560" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2561">
+      <c r="A2561" s="1" t="n">
+        <v>43998.5240702199</v>
+      </c>
+      <c r="B2561" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2561" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2561" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2561" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2561" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2561" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2561" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2561" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2562">
+      <c r="A2562" s="1" t="n">
+        <v>43998.5341318866</v>
+      </c>
+      <c r="B2562" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2562" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2562" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2562" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2562" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2562" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2562" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2562" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2563">
+      <c r="A2563" s="1" t="n">
+        <v>43998.6358371412</v>
+      </c>
+      <c r="B2563" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2563" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2563" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2563" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2563" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2563" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2563" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2563" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2564">
+      <c r="A2564" s="1" t="n">
+        <v>43998.7873412847</v>
+      </c>
+      <c r="B2564" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2564" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2564" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2564" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2564" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2564" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2564" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2564" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2565">
+      <c r="A2565" s="1" t="n">
+        <v>43998.7886924421</v>
+      </c>
+      <c r="B2565" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2565" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2565" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2565" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2565" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2565" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2565" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2565" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2566">
+      <c r="A2566" s="1" t="n">
+        <v>43998.9732069792</v>
+      </c>
+      <c r="B2566" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2566" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2566" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2566" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2566" t="n">
+        <v>61</v>
+      </c>
+      <c r="G2566" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2566" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2566" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2567">
+      <c r="A2567" s="1" t="n">
+        <v>43998.9732466319</v>
+      </c>
+      <c r="B2567" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2567" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2567" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2567" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2567" t="n">
+        <v>62</v>
+      </c>
+      <c r="G2567" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2567" t="n">
+        <v>18</v>
+      </c>
+      <c r="I2567" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2568">
+      <c r="A2568" s="1" t="n">
+        <v>43999.3388856597</v>
+      </c>
+      <c r="B2568" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2568" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2568" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2568" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2568" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2568" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2568" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2568" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2569">
+      <c r="A2569" s="1" t="n">
+        <v>43999.3575567708</v>
+      </c>
+      <c r="B2569" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2569" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2569" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2569" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2569" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2569" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2569" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2569" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2570">
+      <c r="A2570" s="1" t="n">
+        <v>43999.3707050926</v>
+      </c>
+      <c r="B2570" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2570" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2570" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2570" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2570" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2570" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2570" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2570" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2571">
+      <c r="A2571" s="1" t="n">
+        <v>43999.3772169097</v>
+      </c>
+      <c r="B2571" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2571" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2571" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2571" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2571" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2571" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2571" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2571" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2572">
+      <c r="A2572" s="1" t="n">
+        <v>43999.386539838</v>
+      </c>
+      <c r="B2572" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2572" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2572" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2572" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2572" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2572" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2572" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2572" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2573">
+      <c r="A2573" s="1" t="n">
+        <v>43999.3872977083</v>
+      </c>
+      <c r="B2573" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2573" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2573" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2573" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2573" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2573" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2573" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2573" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2574">
+      <c r="A2574" s="1" t="n">
+        <v>43999.3892715972</v>
+      </c>
+      <c r="B2574" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2574" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2574" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2574" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2574" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2574" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2574" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2574" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2575">
+      <c r="A2575" s="1" t="n">
+        <v>43999.3914273958</v>
+      </c>
+      <c r="B2575" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2575" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2575" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2575" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2575" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2575" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2575" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2575" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2576">
+      <c r="A2576" s="1" t="n">
+        <v>43999.3917195602</v>
+      </c>
+      <c r="B2576" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2576" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2576" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2576" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2576" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2576" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2576" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2576" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2577">
+      <c r="A2577" s="1" t="n">
+        <v>43999.397225382</v>
+      </c>
+      <c r="B2577" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2577" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2577" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2577" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2577" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2577" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2577" t="n">
+        <v>33</v>
+      </c>
+      <c r="I2577" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2578">
+      <c r="A2578" s="1" t="n">
+        <v>43999.3977569097</v>
+      </c>
+      <c r="B2578" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2578" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2578" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2578" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2578" t="n">
+        <v>90</v>
+      </c>
+      <c r="G2578" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2578" t="n">
+        <v>34</v>
+      </c>
+      <c r="I2578" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2579">
+      <c r="A2579" s="1" t="n">
+        <v>43999.3984471643</v>
+      </c>
+      <c r="B2579" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2579" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2579" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2579" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2579" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2579" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2579" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2579" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2580">
+      <c r="A2580" s="1" t="n">
+        <v>43999.4162062153</v>
+      </c>
+      <c r="B2580" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2580" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2580" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2580" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2580" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2580" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2580" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2580" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2581">
+      <c r="A2581" s="1" t="n">
+        <v>43999.4314869213</v>
+      </c>
+      <c r="B2581" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2581" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2581" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2581" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2581" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2581" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2581" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2581" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2582">
+      <c r="A2582" s="1" t="n">
+        <v>43999.4322702431</v>
+      </c>
+      <c r="B2582" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2582" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2582" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2582" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2582" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2582" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2582" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2582" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2583">
+      <c r="A2583" s="1" t="n">
+        <v>43999.4419186343</v>
+      </c>
+      <c r="B2583" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2583" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2583" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2583" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2583" t="n">
+        <v>64</v>
+      </c>
+      <c r="G2583" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2583" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2583" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2584">
+      <c r="A2584" s="1" t="n">
+        <v>43999.4420062963</v>
+      </c>
+      <c r="B2584" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2584" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2584" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2584" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2584" t="n">
+        <v>64</v>
+      </c>
+      <c r="G2584" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2584" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2584" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2585">
+      <c r="A2585" s="1" t="n">
+        <v>43999.4595820833</v>
+      </c>
+      <c r="B2585" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2585" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2585" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2585" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2585" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2585" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2585" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2585" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2586">
+      <c r="A2586" s="1" t="n">
+        <v>43999.4723376389</v>
+      </c>
+      <c r="B2586" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2586" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2586" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2586" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2586" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2586" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2586" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2586" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2587">
+      <c r="A2587" s="1" t="n">
+        <v>43999.4762001852</v>
+      </c>
+      <c r="B2587" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2587" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2587" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2587" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2587" t="n">
+        <v>78</v>
+      </c>
+      <c r="G2587" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2587" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2587" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2588">
+      <c r="A2588" s="1" t="n">
+        <v>43999.4773389815</v>
+      </c>
+      <c r="B2588" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2588" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2588" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2588" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2588" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2588" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2588" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2588" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2589">
+      <c r="A2589" s="1" t="n">
+        <v>43999.4834154977</v>
+      </c>
+      <c r="B2589" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2589" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2589" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2589" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2589" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2589" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2589" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2589" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2590">
+      <c r="A2590" s="1" t="n">
+        <v>43999.5006767245</v>
+      </c>
+      <c r="B2590" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2590" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2590" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2590" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2590" t="n">
+        <v>49</v>
+      </c>
+      <c r="G2590" t="n">
+        <v>11</v>
+      </c>
+      <c r="H2590" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2590" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2591">
+      <c r="A2591" s="1" t="n">
+        <v>43999.5009315972</v>
+      </c>
+      <c r="B2591" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2591" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2591" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2591" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2591" t="n">
+        <v>78</v>
+      </c>
+      <c r="G2591" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2591" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2591" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2592">
+      <c r="A2592" s="1" t="n">
+        <v>43999.5104625926</v>
+      </c>
+      <c r="B2592" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2592" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2592" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2592" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2592" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2592" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2592" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2592" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2593">
+      <c r="A2593" s="1" t="n">
+        <v>43999.5173392245</v>
+      </c>
+      <c r="B2593" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2593" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2593" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2593" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2593" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2593" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2593" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2593" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2594">
+      <c r="A2594" s="1" t="n">
+        <v>43999.5508936111</v>
+      </c>
+      <c r="B2594" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2594" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2594" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2594" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2594" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2594" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2594" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2594" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2595">
+      <c r="A2595" s="1" t="n">
+        <v>43999.5627965278</v>
+      </c>
+      <c r="B2595" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2595" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2595" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2595" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2595" t="n">
+        <v>64</v>
+      </c>
+      <c r="G2595" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2595" t="n">
+        <v>17</v>
+      </c>
+      <c r="I2595" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2596">
+      <c r="A2596" s="1" t="n">
+        <v>43999.5863543981</v>
+      </c>
+      <c r="B2596" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2596" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2596" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2596" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2596" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2596" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2596" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2596" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2597">
+      <c r="A2597" s="1" t="n">
+        <v>43999.8015153125</v>
+      </c>
+      <c r="B2597" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2597" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2597" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2597" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2597" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2597" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2597" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2597" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2598">
+      <c r="A2598" s="1" t="n">
+        <v>43999.801684537</v>
+      </c>
+      <c r="B2598" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2598" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2598" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2598" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2598" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2598" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2598" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2598" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2599">
+      <c r="A2599" s="1" t="n">
+        <v>43999.847598588</v>
+      </c>
+      <c r="B2599" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2599" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2599" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2599" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2599" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2599" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2599" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2599" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2600">
+      <c r="A2600" s="1" t="n">
+        <v>44000.0481841435</v>
+      </c>
+      <c r="B2600" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2600" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2600" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2600" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2600" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2600" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2600" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2600" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2601">
+      <c r="A2601" s="1" t="n">
+        <v>44000.049204537</v>
+      </c>
+      <c r="B2601" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2601" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2601" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2601" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2601" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2601" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2601" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2601" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2602">
+      <c r="A2602" s="1" t="n">
+        <v>44000.3331687616</v>
+      </c>
+      <c r="B2602" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2602" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2602" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2602" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2602" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2602" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2602" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2602" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2603">
+      <c r="A2603" s="1" t="n">
+        <v>44000.3348065625</v>
+      </c>
+      <c r="B2603" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2603" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2603" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2603" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2603" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2603" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2603" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2603" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2604">
+      <c r="A2604" s="1" t="n">
+        <v>44000.3412594329</v>
+      </c>
+      <c r="B2604" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2604" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2604" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2604" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2604" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2604" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2604" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2604" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2605">
+      <c r="A2605" s="1" t="n">
+        <v>44000.3462686574</v>
+      </c>
+      <c r="B2605" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2605" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2605" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2605" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2605" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2605" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2605" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2605" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2606">
+      <c r="A2606" s="1" t="n">
+        <v>44000.3565367477</v>
+      </c>
+      <c r="B2606" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2606" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2606" t="n">
+        <v>112</v>
+      </c>
+      <c r="E2606" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2606" t="n">
+        <v>90</v>
+      </c>
+      <c r="G2606" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2606" t="n">
+        <v>34</v>
+      </c>
+      <c r="I2606" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2607">
+      <c r="A2607" s="1" t="n">
+        <v>44000.3579607407</v>
+      </c>
+      <c r="B2607" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2607" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2607" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2607" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2607" t="n">
+        <v>93</v>
+      </c>
+      <c r="G2607" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2607" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2607" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2608">
+      <c r="A2608" s="1" t="n">
+        <v>44000.3622406366</v>
+      </c>
+      <c r="B2608" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2608" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2608" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2608" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2608" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2608" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2608" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2608" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2609">
+      <c r="A2609" s="1" t="n">
+        <v>44000.3649219676</v>
+      </c>
+      <c r="B2609" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2609" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2609" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2609" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2609" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2609" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2609" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2609" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2610">
+      <c r="A2610" s="1" t="n">
+        <v>44000.3744887616</v>
+      </c>
+      <c r="B2610" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2610" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2610" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2610" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2610" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2610" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2610" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2610" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2611">
+      <c r="A2611" s="1" t="n">
+        <v>44000.3925516898</v>
+      </c>
+      <c r="B2611" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2611" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2611" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2611" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2611" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2611" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2611" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2611" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2612">
+      <c r="A2612" s="1" t="n">
+        <v>44000.3937099074</v>
+      </c>
+      <c r="B2612" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2612" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2612" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2612" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2612" t="n">
+        <v>47</v>
+      </c>
+      <c r="G2612" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2612" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2612" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2613">
+      <c r="A2613" s="1" t="n">
+        <v>44000.3972667708</v>
+      </c>
+      <c r="B2613" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2613" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2613" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2613" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2613" t="n">
+        <v>62</v>
+      </c>
+      <c r="G2613" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2613" t="n">
+        <v>16</v>
+      </c>
+      <c r="I2613" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2614">
+      <c r="A2614" s="1" t="n">
+        <v>44000.4069544676</v>
+      </c>
+      <c r="B2614" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2614" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2614" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2614" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2614" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2614" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2614" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2614" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2615">
+      <c r="A2615" s="1" t="n">
+        <v>44000.4264652893</v>
+      </c>
+      <c r="B2615" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2615" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2615" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2615" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2615" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2615" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2615" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2615" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2616">
+      <c r="A2616" s="1" t="n">
+        <v>44000.4271234491</v>
+      </c>
+      <c r="B2616" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2616" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2616" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2616" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2616" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2616" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2616" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2616" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2617">
+      <c r="A2617" s="1" t="n">
+        <v>44000.4317773264</v>
+      </c>
+      <c r="B2617" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2617" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2617" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2617" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2617" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2617" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2617" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2617" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2618">
+      <c r="A2618" s="1" t="n">
+        <v>44000.4467809838</v>
+      </c>
+      <c r="B2618" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2618" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2618" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2618" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2618" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2618" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2618" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2618" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2619">
+      <c r="A2619" s="1" t="n">
+        <v>44000.4775267014</v>
+      </c>
+      <c r="B2619" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2619" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2619" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2619" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2619" t="n">
+        <v>74</v>
+      </c>
+      <c r="G2619" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2619" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2619" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2620">
+      <c r="A2620" s="1" t="n">
+        <v>44000.4787066667</v>
+      </c>
+      <c r="B2620" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2620" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2620" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2620" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2620" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2620" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2620" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2620" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2621">
+      <c r="A2621" s="1" t="n">
+        <v>44000.5525189815</v>
+      </c>
+      <c r="B2621" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2621" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2621" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2621" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2621" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2621" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2621" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2621" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2622">
+      <c r="A2622" s="1" t="n">
+        <v>44000.558443588</v>
+      </c>
+      <c r="B2622" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2622" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2622" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2622" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2622" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2622" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2622" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2622" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2623">
+      <c r="A2623" s="1" t="n">
+        <v>44000.6233570718</v>
+      </c>
+      <c r="B2623" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2623" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2623" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2623" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2623" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2623" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2623" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2623" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2624">
+      <c r="A2624" s="1" t="n">
+        <v>44000.6516970949</v>
+      </c>
+      <c r="B2624" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2624" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2624" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2624" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2624" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2624" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2624" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2624" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2625">
+      <c r="A2625" s="1" t="n">
+        <v>44000.6525436574</v>
+      </c>
+      <c r="B2625" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2625" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2625" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2625" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2625" t="n">
+        <v>62</v>
+      </c>
+      <c r="G2625" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2625" t="n">
+        <v>16</v>
+      </c>
+      <c r="I2625" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2626">
+      <c r="A2626" s="1" t="n">
+        <v>44000.724633287</v>
+      </c>
+      <c r="B2626" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2626" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2626" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2626" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2626" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2626" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2626" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2626" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2627">
+      <c r="A2627" s="1" t="n">
+        <v>44000.7599690741</v>
+      </c>
+      <c r="B2627" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2627" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2627" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2627" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2627" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2627" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2627" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2627" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2628">
+      <c r="A2628" s="1" t="n">
+        <v>44000.7930978472</v>
+      </c>
+      <c r="B2628" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2628" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2628" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2628" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2628" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2628" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2628" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2628" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2629">
+      <c r="A2629" s="1" t="n">
+        <v>44000.8204519907</v>
+      </c>
+      <c r="B2629" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2629" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2629" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2629" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2629" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2629" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2629" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2629" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2630">
+      <c r="A2630" s="1" t="n">
+        <v>44000.900862963</v>
+      </c>
+      <c r="B2630" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2630" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2630" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2630" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2630" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2630" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2630" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2630" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2631">
+      <c r="A2631" s="1" t="n">
+        <v>44000.9009080903</v>
+      </c>
+      <c r="B2631" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2631" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2631" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2631" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2631" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2631" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2631" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2631" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2632">
+      <c r="A2632" s="1" t="n">
+        <v>44001.0176983912</v>
+      </c>
+      <c r="B2632" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2632" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2632" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2632" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2632" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2632" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2632" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2632" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2633">
+      <c r="A2633" s="1" t="n">
+        <v>44001.1639487384</v>
+      </c>
+      <c r="B2633" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2633" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2633" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2633" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2633" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2633" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2633" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2633" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2634">
+      <c r="A2634" s="1" t="n">
+        <v>44001.3634200347</v>
+      </c>
+      <c r="B2634" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2634" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2634" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2634" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2634" t="n">
+        <v>93</v>
+      </c>
+      <c r="G2634" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2634" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2634" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2635">
+      <c r="A2635" s="1" t="n">
+        <v>44001.3644917361</v>
+      </c>
+      <c r="B2635" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2635" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2635" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2635" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2635" t="n">
+        <v>97</v>
+      </c>
+      <c r="G2635" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2635" t="n">
+        <v>38</v>
+      </c>
+      <c r="I2635" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2636">
+      <c r="A2636" s="1" t="n">
+        <v>44001.3706596412</v>
+      </c>
+      <c r="B2636" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2636" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2636" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2636" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2636" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2636" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2636" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2636" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2637">
+      <c r="A2637" s="1" t="n">
+        <v>44001.3734110417</v>
+      </c>
+      <c r="B2637" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2637" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2637" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2637" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2637" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2637" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2637" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2637" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2638">
+      <c r="A2638" s="1" t="n">
+        <v>44001.3750530093</v>
+      </c>
+      <c r="B2638" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2638" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2638" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2638" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2638" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2638" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2638" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2638" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2639">
+      <c r="A2639" s="1" t="n">
+        <v>44001.3896110185</v>
+      </c>
+      <c r="B2639" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2639" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2639" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2639" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2639" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2639" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2639" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2639" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2640">
+      <c r="A2640" s="1" t="n">
+        <v>44001.3925559028</v>
+      </c>
+      <c r="B2640" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2640" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2640" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2640" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2640" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2640" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2640" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2640" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2641">
+      <c r="A2641" s="1" t="n">
+        <v>44001.3943398843</v>
+      </c>
+      <c r="B2641" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2641" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2641" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2641" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2641" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2641" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2641" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2641" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2642">
+      <c r="A2642" s="1" t="n">
+        <v>44001.3952228704</v>
+      </c>
+      <c r="B2642" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2642" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2642" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2642" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2642" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2642" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2642" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2642" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2643">
+      <c r="A2643" s="1" t="n">
+        <v>44001.3962278241</v>
+      </c>
+      <c r="B2643" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2643" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2643" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2643" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2643" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2643" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2643" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2643" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2644">
+      <c r="A2644" s="1" t="n">
+        <v>44001.401642963</v>
+      </c>
+      <c r="B2644" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2644" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2644" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2644" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2644" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2644" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2644" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2644" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2645">
+      <c r="A2645" s="1" t="n">
+        <v>44001.4127983681</v>
+      </c>
+      <c r="B2645" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2645" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2645" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2645" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2645" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2645" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2645" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2645" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2646">
+      <c r="A2646" s="1" t="n">
+        <v>44001.4128021759</v>
+      </c>
+      <c r="B2646" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2646" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2646" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2646" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2646" t="n">
+        <v>44</v>
+      </c>
+      <c r="G2646" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2646" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2646" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2647">
+      <c r="A2647" s="1" t="n">
+        <v>44001.4128209259</v>
+      </c>
+      <c r="B2647" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2647" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2647" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2647" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2647" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2647" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2647" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2647" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2648">
+      <c r="A2648" s="1" t="n">
+        <v>44001.4129415741</v>
+      </c>
+      <c r="B2648" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2648" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2648" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2648" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2648" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2648" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2648" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2648" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2649">
+      <c r="A2649" s="1" t="n">
+        <v>44001.412948588</v>
+      </c>
+      <c r="B2649" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2649" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2649" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2649" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2649" t="n">
+        <v>49</v>
+      </c>
+      <c r="G2649" t="n">
+        <v>11</v>
+      </c>
+      <c r="H2649" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2649" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2650">
+      <c r="A2650" s="1" t="n">
+        <v>44001.4129802893</v>
+      </c>
+      <c r="B2650" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2650" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2650" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2650" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2650" t="n">
+        <v>44</v>
+      </c>
+      <c r="G2650" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2650" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2650" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2651">
+      <c r="A2651" s="1" t="n">
+        <v>44001.4130062037</v>
+      </c>
+      <c r="B2651" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2651" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2651" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2651" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2651" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2651" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2651" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2651" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2652">
+      <c r="A2652" s="1" t="n">
+        <v>44001.413039213</v>
+      </c>
+      <c r="B2652" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2652" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2652" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2652" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2652" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2652" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2652" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2652" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2653">
+      <c r="A2653" s="1" t="n">
+        <v>44001.4203955903</v>
+      </c>
+      <c r="B2653" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2653" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2653" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2653" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2653" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2653" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2653" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2653" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2654">
+      <c r="A2654" s="1" t="n">
+        <v>44001.4243856481</v>
+      </c>
+      <c r="B2654" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2654" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2654" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2654" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2654" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2654" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2654" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2654" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2655">
+      <c r="A2655" s="1" t="n">
+        <v>44001.4327584259</v>
+      </c>
+      <c r="B2655" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2655" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2655" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2655" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2655" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2655" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2655" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2655" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Acrescentado Shinithemes Antes de tentar colocar a escala linear
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -412,6 +412,9 @@
   <si>
     <t xml:space="preserve">Hlanziotti@gmail.com</t>
   </si>
+  <si>
+    <t xml:space="preserve">taianivargad@hotmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -77745,6 +77748,1224 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2656">
+      <c r="A2656" s="1" t="n">
+        <v>44001.4587975</v>
+      </c>
+      <c r="B2656" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2656" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2656" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2656" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2656" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2656" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2656" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2656" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2657">
+      <c r="A2657" s="1" t="n">
+        <v>44001.4969082986</v>
+      </c>
+      <c r="B2657" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2657" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2657" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2657" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2657" t="n">
+        <v>69</v>
+      </c>
+      <c r="G2657" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2657" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2657" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2658">
+      <c r="A2658" s="1" t="n">
+        <v>44001.4977388079</v>
+      </c>
+      <c r="B2658" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2658" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2658" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2658" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2658" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2658" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2658" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2658" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2659">
+      <c r="A2659" s="1" t="n">
+        <v>44001.5071293519</v>
+      </c>
+      <c r="B2659" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2659" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2659" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2659" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2659" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2659" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2659" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2659" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2660">
+      <c r="A2660" s="1" t="n">
+        <v>44001.5600644329</v>
+      </c>
+      <c r="B2660" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2660" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2660" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2660" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2660" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2660" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2660" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2660" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2661">
+      <c r="A2661" s="1" t="n">
+        <v>44001.5605259722</v>
+      </c>
+      <c r="B2661" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2661" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2661" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2661" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2661" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2661" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2661" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2661" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2662">
+      <c r="A2662" s="1" t="n">
+        <v>44001.5878303009</v>
+      </c>
+      <c r="B2662" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2662" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2662" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2662" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2662" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2662" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2662" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2662" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2663">
+      <c r="A2663" s="1" t="n">
+        <v>44001.6375027894</v>
+      </c>
+      <c r="B2663" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2663" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2663" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2663" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2663" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2663" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2663" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2663" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2664">
+      <c r="A2664" s="1" t="n">
+        <v>44001.6784255671</v>
+      </c>
+      <c r="B2664" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2664" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2664" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2664" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2664" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2664" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2664" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2664" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2665">
+      <c r="A2665" s="1" t="n">
+        <v>44001.6873026157</v>
+      </c>
+      <c r="B2665" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2665" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2665" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2665" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2665" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2665" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2665" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2665" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2666">
+      <c r="A2666" s="1" t="n">
+        <v>44001.7217681019</v>
+      </c>
+      <c r="B2666" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2666" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2666" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2666" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2666" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2666" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2666" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2666" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2667">
+      <c r="A2667" s="1" t="n">
+        <v>44001.7219416088</v>
+      </c>
+      <c r="B2667" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2667" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2667" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2667" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2667" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2667" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2667" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2667" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2668">
+      <c r="A2668" s="1" t="n">
+        <v>44001.7233820949</v>
+      </c>
+      <c r="B2668" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2668" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2668" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2668" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2668" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2668" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2668" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2668" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2669">
+      <c r="A2669" s="1" t="n">
+        <v>44001.7235947222</v>
+      </c>
+      <c r="B2669" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2669" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2669" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2669" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2669" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2669" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2669" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2669" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2670">
+      <c r="A2670" s="1" t="n">
+        <v>44001.7242786227</v>
+      </c>
+      <c r="B2670" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2670" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2670" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2670" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2670" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2670" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2670" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2670" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2671">
+      <c r="A2671" s="1" t="n">
+        <v>44001.7243982639</v>
+      </c>
+      <c r="B2671" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2671" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2671" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2671" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2671" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2671" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2671" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2671" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2672">
+      <c r="A2672" s="1" t="n">
+        <v>44001.7256667014</v>
+      </c>
+      <c r="B2672" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2672" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2672" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2672" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2672" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2672" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2672" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2672" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2673">
+      <c r="A2673" s="1" t="n">
+        <v>44001.7257756482</v>
+      </c>
+      <c r="B2673" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2673" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2673" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2673" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2673" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2673" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2673" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2673" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2674">
+      <c r="A2674" s="1" t="n">
+        <v>44001.7349621412</v>
+      </c>
+      <c r="B2674" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2674" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2674" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2674" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2674" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2674" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2674" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2674" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2675">
+      <c r="A2675" s="1" t="n">
+        <v>44001.735082338</v>
+      </c>
+      <c r="B2675" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2675" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2675" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2675" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2675" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2675" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2675" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2675" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2676">
+      <c r="A2676" s="1" t="n">
+        <v>44001.7356382176</v>
+      </c>
+      <c r="B2676" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2676" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2676" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2676" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2676" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2676" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2676" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2676" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2677">
+      <c r="A2677" s="1" t="n">
+        <v>44001.7383912153</v>
+      </c>
+      <c r="B2677" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2677" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2677" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2677" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2677" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2677" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2677" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2677" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2678">
+      <c r="A2678" s="1" t="n">
+        <v>44001.7709613889</v>
+      </c>
+      <c r="B2678" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2678" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2678" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2678" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2678" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2678" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2678" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2678" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2679">
+      <c r="A2679" s="1" t="n">
+        <v>44001.8073495023</v>
+      </c>
+      <c r="B2679" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2679" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2679" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2679" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2679" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2679" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2679" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2679" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2680">
+      <c r="A2680" s="1" t="n">
+        <v>44001.8103806944</v>
+      </c>
+      <c r="B2680" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2680" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2680" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2680" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2680" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2680" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2680" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2680" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2681">
+      <c r="A2681" s="1" t="n">
+        <v>44001.8465621065</v>
+      </c>
+      <c r="B2681" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2681" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2681" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2681" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2681" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2681" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2681" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2681" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2682">
+      <c r="A2682" s="1" t="n">
+        <v>44002.064219213</v>
+      </c>
+      <c r="B2682" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2682" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2682" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2682" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2682" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2682" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2682" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2682" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2683">
+      <c r="A2683" s="1" t="n">
+        <v>44002.3248381134</v>
+      </c>
+      <c r="B2683" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2683" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2683" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2683" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2683" t="n">
+        <v>49</v>
+      </c>
+      <c r="G2683" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2683" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2683" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2684">
+      <c r="A2684" s="1" t="n">
+        <v>44002.3618189468</v>
+      </c>
+      <c r="B2684" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2684" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2684" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2684" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2684" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2684" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2684" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2684" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2685">
+      <c r="A2685" s="1" t="n">
+        <v>44002.3751276042</v>
+      </c>
+      <c r="B2685" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2685" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2685" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2685" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2685" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2685" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2685" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2685" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2686">
+      <c r="A2686" s="1" t="n">
+        <v>44002.3763680093</v>
+      </c>
+      <c r="B2686" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2686" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2686" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2686" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2686" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2686" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2686" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2686" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2687">
+      <c r="A2687" s="1" t="n">
+        <v>44002.3826608102</v>
+      </c>
+      <c r="B2687" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2687" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2687" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2687" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2687" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2687" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2687" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2687" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2688">
+      <c r="A2688" s="1" t="n">
+        <v>44002.3893542477</v>
+      </c>
+      <c r="B2688" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2688" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2688" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2688" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2688" t="n">
+        <v>97</v>
+      </c>
+      <c r="G2688" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2688" t="n">
+        <v>38</v>
+      </c>
+      <c r="I2688" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2689">
+      <c r="A2689" s="1" t="n">
+        <v>44002.3895087153</v>
+      </c>
+      <c r="B2689" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2689" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2689" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2689" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2689" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2689" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2689" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2689" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2690">
+      <c r="A2690" s="1" t="n">
+        <v>44002.3904060764</v>
+      </c>
+      <c r="B2690" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2690" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2690" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2690" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2690" t="n">
+        <v>98</v>
+      </c>
+      <c r="G2690" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2690" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2690" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2691">
+      <c r="A2691" s="1" t="n">
+        <v>44002.391707037</v>
+      </c>
+      <c r="B2691" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2691" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2691" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2691" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2691" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2691" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2691" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2691" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2692">
+      <c r="A2692" s="1" t="n">
+        <v>44002.3983591667</v>
+      </c>
+      <c r="B2692" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2692" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2692" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2692" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2692" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2692" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2692" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2692" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2693">
+      <c r="A2693" s="1" t="n">
+        <v>44002.4260890393</v>
+      </c>
+      <c r="B2693" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2693" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2693" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2693" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2693" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2693" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2693" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2693" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2694">
+      <c r="A2694" s="1" t="n">
+        <v>44002.439876412</v>
+      </c>
+      <c r="B2694" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2694" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2694" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2694" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2694" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2694" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2694" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2694" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2695">
+      <c r="A2695" s="1" t="n">
+        <v>44002.4491817361</v>
+      </c>
+      <c r="B2695" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2695" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2695" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2695" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2695" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2695" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2695" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2695" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2696">
+      <c r="A2696" s="1" t="n">
+        <v>44002.4541492708</v>
+      </c>
+      <c r="B2696" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2696" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2696" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2696" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2696" t="n">
+        <v>98</v>
+      </c>
+      <c r="G2696" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2696" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2696" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2697">
+      <c r="A2697" s="1" t="n">
+        <v>44002.4600214352</v>
+      </c>
+      <c r="B2697" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2697" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2697" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2697" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2697" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2697" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2697" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2697" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Ajustada a altura da janela de regressão
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -78966,6 +78966,383 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2698">
+      <c r="A2698" s="1" t="n">
+        <v>44002.4747277662</v>
+      </c>
+      <c r="B2698" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2698" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2698" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2698" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2698" t="n">
+        <v>67</v>
+      </c>
+      <c r="G2698" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2698" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2698" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2699">
+      <c r="A2699" s="1" t="n">
+        <v>44002.4758911343</v>
+      </c>
+      <c r="B2699" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2699" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2699" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2699" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2699" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2699" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2699" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2699" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2700">
+      <c r="A2700" s="1" t="n">
+        <v>44002.4786225</v>
+      </c>
+      <c r="B2700" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2700" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2700" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2700" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2700" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2700" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2700" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2700" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2701">
+      <c r="A2701" s="1" t="n">
+        <v>44002.4792671875</v>
+      </c>
+      <c r="B2701" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2701" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2701" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2701" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2701" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2701" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2701" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2701" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2702">
+      <c r="A2702" s="1" t="n">
+        <v>44002.5913029745</v>
+      </c>
+      <c r="B2702" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2702" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2702" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2702" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2702" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2702" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2702" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2702" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2703">
+      <c r="A2703" s="1" t="n">
+        <v>44002.6254537731</v>
+      </c>
+      <c r="B2703" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2703" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2703" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2703" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2703" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2703" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2703" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2703" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2704">
+      <c r="A2704" s="1" t="n">
+        <v>44002.6584331366</v>
+      </c>
+      <c r="B2704" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2704" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2704" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2704" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2704" t="n">
+        <v>68</v>
+      </c>
+      <c r="G2704" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2704" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2704" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2705">
+      <c r="A2705" s="1" t="n">
+        <v>44002.6967789815</v>
+      </c>
+      <c r="B2705" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2705" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2705" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2705" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2705" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2705" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2705" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2705" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2706">
+      <c r="A2706" s="1" t="n">
+        <v>44002.7184389699</v>
+      </c>
+      <c r="B2706" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2706" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2706" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2706" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2706" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2706" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2706" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2706" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2707">
+      <c r="A2707" s="1" t="n">
+        <v>44002.7189697338</v>
+      </c>
+      <c r="B2707" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2707" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2707" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2707" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2707" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2707" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2707" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2707" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2708">
+      <c r="A2708" s="1" t="n">
+        <v>44002.7532172685</v>
+      </c>
+      <c r="B2708" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2708" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2708" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2708" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2708" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2708" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2708" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2708" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2709">
+      <c r="A2709" s="1" t="n">
+        <v>44002.7856782639</v>
+      </c>
+      <c r="B2709" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2709" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2709" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2709" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2709" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2709" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2709" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2709" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2710">
+      <c r="A2710" s="1" t="n">
+        <v>44002.7912107407</v>
+      </c>
+      <c r="B2710" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2710" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2710" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2710" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2710" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2710" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2710" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2710" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Retirada de linhas não utilizadas
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -79343,6 +79343,122 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2711">
+      <c r="A2711" s="1" t="n">
+        <v>44002.8473634375</v>
+      </c>
+      <c r="B2711" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2711" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2711" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2711" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2711" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2711" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2711" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2711" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2712">
+      <c r="A2712" s="1" t="n">
+        <v>44002.8514509954</v>
+      </c>
+      <c r="B2712" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2712" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2712" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2712" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2712" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2712" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2712" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2712" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2713">
+      <c r="A2713" s="1" t="n">
+        <v>44002.9120465856</v>
+      </c>
+      <c r="B2713" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2713" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2713" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2713" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2713" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2713" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2713" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2713" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2714">
+      <c r="A2714" s="1" t="n">
+        <v>44003.0137049884</v>
+      </c>
+      <c r="B2714" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2714" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2714" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2714" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2714" t="n">
+        <v>68</v>
+      </c>
+      <c r="G2714" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2714" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2714" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Acrescentado a diferença percentual no gráfico
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -79459,6 +79459,122 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2715">
+      <c r="A2715" s="1" t="n">
+        <v>44003.0756574421</v>
+      </c>
+      <c r="B2715" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2715" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2715" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2715" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2715" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2715" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2715" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2715" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2716">
+      <c r="A2716" s="1" t="n">
+        <v>44003.0758843866</v>
+      </c>
+      <c r="B2716" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2716" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2716" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2716" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2716" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2716" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2716" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2716" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2717">
+      <c r="A2717" s="1" t="n">
+        <v>44003.3144454514</v>
+      </c>
+      <c r="B2717" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2717" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2717" t="n">
+        <v>118</v>
+      </c>
+      <c r="E2717" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2717" t="n">
+        <v>98</v>
+      </c>
+      <c r="G2717" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2717" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2717" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2718">
+      <c r="A2718" s="1" t="n">
+        <v>44003.3156080903</v>
+      </c>
+      <c r="B2718" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2718" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2718" t="n">
+        <v>123</v>
+      </c>
+      <c r="E2718" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2718" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2718" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2718" t="n">
+        <v>38</v>
+      </c>
+      <c r="I2718" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Atualização dos dados somente
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -415,6 +415,9 @@
   <si>
     <t xml:space="preserve">taianivargad@hotmail.com</t>
   </si>
+  <si>
+    <t xml:space="preserve">andre.machado@hed.com.combr</t>
+  </si>
 </sst>
 </file>
 
@@ -79575,6 +79578,731 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2719">
+      <c r="A2719" s="1" t="n">
+        <v>44003.3510917824</v>
+      </c>
+      <c r="B2719" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2719" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2719" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2719" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2719" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2719" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2719" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2719" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2720">
+      <c r="A2720" s="1" t="n">
+        <v>44003.371575</v>
+      </c>
+      <c r="B2720" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2720" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2720" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2720" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2720" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2720" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2720" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2720" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2721">
+      <c r="A2721" s="1" t="n">
+        <v>44003.3931987384</v>
+      </c>
+      <c r="B2721" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2721" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2721" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2721" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2721" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2721" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2721" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2721" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2722">
+      <c r="A2722" s="1" t="n">
+        <v>44003.403797963</v>
+      </c>
+      <c r="B2722" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2722" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2722" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2722" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2722" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2722" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2722" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2722" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2723">
+      <c r="A2723" s="1" t="n">
+        <v>44003.4072846412</v>
+      </c>
+      <c r="B2723" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2723" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2723" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2723" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2723" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2723" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2723" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2723" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2724">
+      <c r="A2724" s="1" t="n">
+        <v>44003.4176154051</v>
+      </c>
+      <c r="B2724" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2724" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2724" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2724" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2724" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2724" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2724" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2724" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2725">
+      <c r="A2725" s="1" t="n">
+        <v>44003.4279219097</v>
+      </c>
+      <c r="B2725" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2725" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2725" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2725" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2725" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2725" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2725" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2725" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2726">
+      <c r="A2726" s="1" t="n">
+        <v>44003.4304133333</v>
+      </c>
+      <c r="B2726" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2726" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2726" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2726" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2726" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2726" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2726" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2726" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2727">
+      <c r="A2727" s="1" t="n">
+        <v>44003.4461923264</v>
+      </c>
+      <c r="B2727" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2727" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2727" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2727" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2727" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2727" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2727" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2727" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2728">
+      <c r="A2728" s="1" t="n">
+        <v>44003.4476869907</v>
+      </c>
+      <c r="B2728" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2728" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2728" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2728" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2728" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2728" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2728" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2728" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2729">
+      <c r="A2729" s="1" t="n">
+        <v>44003.4598989005</v>
+      </c>
+      <c r="B2729" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2729" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2729" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2729" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2729" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2729" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2729" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2729" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2730">
+      <c r="A2730" s="1" t="n">
+        <v>44003.4716588426</v>
+      </c>
+      <c r="B2730" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2730" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2730" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2730" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2730" t="n">
+        <v>62</v>
+      </c>
+      <c r="G2730" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2730" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2730" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2731">
+      <c r="A2731" s="1" t="n">
+        <v>44003.4735665741</v>
+      </c>
+      <c r="B2731" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2731" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2731" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2731" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2731" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2731" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2731" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2731" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2732">
+      <c r="A2732" s="1" t="n">
+        <v>44003.5096934954</v>
+      </c>
+      <c r="B2732" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2732" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2732" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2732" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2732" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2732" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2732" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2732" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2733">
+      <c r="A2733" s="1" t="n">
+        <v>44003.5123557292</v>
+      </c>
+      <c r="B2733" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2733" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2733" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2733" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2733" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2733" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2733" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2733" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2734">
+      <c r="A2734" s="1" t="n">
+        <v>44003.5164422917</v>
+      </c>
+      <c r="B2734" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2734" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2734" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2734" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2734" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2734" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2734" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2734" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2735">
+      <c r="A2735" s="1" t="n">
+        <v>44003.5280437037</v>
+      </c>
+      <c r="B2735" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2735" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2735" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2735" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2735" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2735" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2735" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2735" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2736">
+      <c r="A2736" s="1" t="n">
+        <v>44003.5518118634</v>
+      </c>
+      <c r="B2736" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2736" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2736" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2736" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2736" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2736" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2736" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2736" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2737">
+      <c r="A2737" s="1" t="n">
+        <v>44003.5697790393</v>
+      </c>
+      <c r="B2737" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2737" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2737" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2737" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2737" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2737" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2737" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2737" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2738">
+      <c r="A2738" s="1" t="n">
+        <v>44003.6433097801</v>
+      </c>
+      <c r="B2738" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2738" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2738" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2738" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2738" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2738" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2738" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2738" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2739">
+      <c r="A2739" s="1" t="n">
+        <v>44003.7831611458</v>
+      </c>
+      <c r="B2739" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2739" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2739" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2739" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2739" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2739" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2739" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2739" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2740">
+      <c r="A2740" s="1" t="n">
+        <v>44003.8265885185</v>
+      </c>
+      <c r="B2740" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2740" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2740" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2740" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2740" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2740" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2740" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2740" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2741">
+      <c r="A2741" s="1" t="n">
+        <v>44004.0422935185</v>
+      </c>
+      <c r="B2741" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2741" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2741" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2741" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2741" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2741" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2741" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2741" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2742">
+      <c r="A2742" s="1" t="n">
+        <v>44004.0429541898</v>
+      </c>
+      <c r="B2742" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2742" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2742" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2742" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2742" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2742" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2742" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2742" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2743">
+      <c r="A2743" s="1" t="n">
+        <v>44004.3060987616</v>
+      </c>
+      <c r="B2743" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2743" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2743" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2743" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2743" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2743" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2743" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2743" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Revisado entrada do ICFUC
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -418,6 +418,9 @@
   <si>
     <t xml:space="preserve">andre.machado@hed.com.combr</t>
   </si>
+  <si>
+    <t xml:space="preserve">renatocvaz@hotmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -80303,6 +80306,1195 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2744">
+      <c r="A2744" s="1" t="n">
+        <v>44004.3257520486</v>
+      </c>
+      <c r="B2744" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2744" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2744" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2744" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2744" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2744" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2744" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2744" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2745">
+      <c r="A2745" s="1" t="n">
+        <v>44004.3372102662</v>
+      </c>
+      <c r="B2745" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2745" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2745" t="n">
+        <v>123</v>
+      </c>
+      <c r="E2745" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2745" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2745" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2745" t="n">
+        <v>38</v>
+      </c>
+      <c r="I2745" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2746">
+      <c r="A2746" s="1" t="n">
+        <v>44004.3381328241</v>
+      </c>
+      <c r="B2746" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2746" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2746" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2746" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2746" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2746" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2746" t="n">
+        <v>43</v>
+      </c>
+      <c r="I2746" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2747">
+      <c r="A2747" s="1" t="n">
+        <v>44004.3435996528</v>
+      </c>
+      <c r="B2747" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2747" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2747" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2747" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2747" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2747" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2747" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2747" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2748">
+      <c r="A2748" s="1" t="n">
+        <v>44004.3455832639</v>
+      </c>
+      <c r="B2748" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2748" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2748" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2748" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2748" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2748" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2748" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2748" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2749">
+      <c r="A2749" s="1" t="n">
+        <v>44004.3843541782</v>
+      </c>
+      <c r="B2749" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2749" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2749" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2749" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2749" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2749" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2749" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2749" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2750">
+      <c r="A2750" s="1" t="n">
+        <v>44004.3897736227</v>
+      </c>
+      <c r="B2750" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2750" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2750" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2750" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2750" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2750" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2750" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2750" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2751">
+      <c r="A2751" s="1" t="n">
+        <v>44004.3924785532</v>
+      </c>
+      <c r="B2751" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2751" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2751" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2751" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2751" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2751" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2751" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2751" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2752">
+      <c r="A2752" s="1" t="n">
+        <v>44004.3996724421</v>
+      </c>
+      <c r="B2752" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2752" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2752" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2752" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2752" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2752" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2752" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2752" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2753">
+      <c r="A2753" s="1" t="n">
+        <v>44004.3997353472</v>
+      </c>
+      <c r="B2753" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2753" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2753" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2753" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2753" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2753" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2753" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2753" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2754">
+      <c r="A2754" s="1" t="n">
+        <v>44004.3997571644</v>
+      </c>
+      <c r="B2754" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2754" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2754" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2754" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2754" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2754" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2754" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2754" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2755">
+      <c r="A2755" s="1" t="n">
+        <v>44004.4164537037</v>
+      </c>
+      <c r="B2755" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2755" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2755" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2755" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2755" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2755" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2755" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2755" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2756">
+      <c r="A2756" s="1" t="n">
+        <v>44004.4196158218</v>
+      </c>
+      <c r="B2756" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2756" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2756" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2756" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2756" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2756" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2756" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2756" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2757">
+      <c r="A2757" s="1" t="n">
+        <v>44004.4255394676</v>
+      </c>
+      <c r="B2757" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2757" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2757" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2757" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2757" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2757" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2757" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2757" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2758">
+      <c r="A2758" s="1" t="n">
+        <v>44004.4264949884</v>
+      </c>
+      <c r="B2758" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2758" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2758" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2758" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2758" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2758" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2758" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2758" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2759">
+      <c r="A2759" s="1" t="n">
+        <v>44004.4270557292</v>
+      </c>
+      <c r="B2759" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2759" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2759" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2759" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2759" t="n">
+        <v>69</v>
+      </c>
+      <c r="G2759" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2759" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2759" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2760">
+      <c r="A2760" s="1" t="n">
+        <v>44004.435489456</v>
+      </c>
+      <c r="B2760" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2760" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2760" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2760" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2760" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2760" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2760" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2760" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2761">
+      <c r="A2761" s="1" t="n">
+        <v>44004.4513226968</v>
+      </c>
+      <c r="B2761" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2761" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2761" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2761" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2761" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2761" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2761" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2761" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2762">
+      <c r="A2762" s="1" t="n">
+        <v>44004.4762848495</v>
+      </c>
+      <c r="B2762" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2762" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2762" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2762" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2762" t="n">
+        <v>70</v>
+      </c>
+      <c r="G2762" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2762" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2762" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2763">
+      <c r="A2763" s="1" t="n">
+        <v>44004.4773660069</v>
+      </c>
+      <c r="B2763" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2763" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2763" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2763" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2763" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2763" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2763" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2763" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2764">
+      <c r="A2764" s="1" t="n">
+        <v>44004.5038592245</v>
+      </c>
+      <c r="B2764" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2764" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2764" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2764" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2764" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2764" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2764" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2764" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2765">
+      <c r="A2765" s="1" t="n">
+        <v>44004.5080246065</v>
+      </c>
+      <c r="B2765" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2765" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2765" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2765" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2765" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2765" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2765" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2765" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2766">
+      <c r="A2766" s="1" t="n">
+        <v>44004.5566112037</v>
+      </c>
+      <c r="B2766" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2766" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2766" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2766" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2766" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2766" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2766" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2766" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2767">
+      <c r="A2767" s="1" t="n">
+        <v>44004.5597599537</v>
+      </c>
+      <c r="B2767" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2767" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2767" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2767" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2767" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2767" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2767" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2767" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2768">
+      <c r="A2768" s="1" t="n">
+        <v>44004.6316032176</v>
+      </c>
+      <c r="B2768" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2768" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2768" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2768" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2768" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2768" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2768" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2768" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2769">
+      <c r="A2769" s="1" t="n">
+        <v>44004.6769332176</v>
+      </c>
+      <c r="B2769" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2769" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2769" t="n">
+        <v>51</v>
+      </c>
+      <c r="E2769" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2769" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2769" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2769" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2769" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2770">
+      <c r="A2770" s="1" t="n">
+        <v>44004.6816339699</v>
+      </c>
+      <c r="B2770" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2770" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2770" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2770" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2770" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2770" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2770" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2770" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2771">
+      <c r="A2771" s="1" t="n">
+        <v>44004.6919118866</v>
+      </c>
+      <c r="B2771" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2771" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2771" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2771" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2771" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2771" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2771" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2771" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2772">
+      <c r="A2772" s="1" t="n">
+        <v>44004.7087064583</v>
+      </c>
+      <c r="B2772" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2772" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2772" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2772" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2772" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2772" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2772" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2772" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2773">
+      <c r="A2773" s="1" t="n">
+        <v>44004.7626814583</v>
+      </c>
+      <c r="B2773" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2773" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2773" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2773" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2773" t="n">
+        <v>41</v>
+      </c>
+      <c r="G2773" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2773" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2773" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2774">
+      <c r="A2774" s="1" t="n">
+        <v>44004.7628308565</v>
+      </c>
+      <c r="B2774" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2774" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2774" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2774" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2774" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2774" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2774" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2774" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2775">
+      <c r="A2775" s="1" t="n">
+        <v>44004.7827978935</v>
+      </c>
+      <c r="B2775" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2775" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2775" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2775" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2775" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2775" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2775" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2775" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2776">
+      <c r="A2776" s="1" t="n">
+        <v>44005.2764640394</v>
+      </c>
+      <c r="B2776" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2776" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2776" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2776" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2776" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2776" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2776" t="n">
+        <v>43</v>
+      </c>
+      <c r="I2776" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2777">
+      <c r="A2777" s="1" t="n">
+        <v>44005.277845463</v>
+      </c>
+      <c r="B2777" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2777" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2777" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2777" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2777" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2777" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2777" t="n">
+        <v>45</v>
+      </c>
+      <c r="I2777" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2778">
+      <c r="A2778" s="1" t="n">
+        <v>44005.3223271181</v>
+      </c>
+      <c r="B2778" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2778" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2778" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2778" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2778" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2778" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2778" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2778" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2779">
+      <c r="A2779" s="1" t="n">
+        <v>44005.3237513889</v>
+      </c>
+      <c r="B2779" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2779" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2779" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2779" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2779" t="n">
+        <v>47</v>
+      </c>
+      <c r="G2779" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2779" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2779" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2780">
+      <c r="A2780" s="1" t="n">
+        <v>44005.3253003241</v>
+      </c>
+      <c r="B2780" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2780" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2780" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2780" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2780" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2780" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2780" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2780" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2781">
+      <c r="A2781" s="1" t="n">
+        <v>44005.3351635648</v>
+      </c>
+      <c r="B2781" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2781" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2781" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2781" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2781" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2781" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2781" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2781" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2782">
+      <c r="A2782" s="1" t="n">
+        <v>44005.379507419</v>
+      </c>
+      <c r="B2782" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2782" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2782" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2782" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2782" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2782" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2782" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2782" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2783">
+      <c r="A2783" s="1" t="n">
+        <v>44005.3822382176</v>
+      </c>
+      <c r="B2783" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2783" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2783" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2783" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2783" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2783" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2783" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2783" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2784">
+      <c r="A2784" s="1" t="n">
+        <v>44005.3836240856</v>
+      </c>
+      <c r="B2784" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2784" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2784" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2784" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2784" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2784" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2784" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2784" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
adicionada a estimativa de erro
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -81495,6 +81495,903 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2785">
+      <c r="A2785" s="1" t="n">
+        <v>44005.404845162</v>
+      </c>
+      <c r="B2785" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2785" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2785" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2785" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2785" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2785" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2785" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2785" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2786">
+      <c r="A2786" s="1" t="n">
+        <v>44005.4218070139</v>
+      </c>
+      <c r="B2786" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2786" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2786" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2786" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2786" t="n">
+        <v>65</v>
+      </c>
+      <c r="G2786" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2786" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2786" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2787">
+      <c r="A2787" s="1" t="n">
+        <v>44005.4317244444</v>
+      </c>
+      <c r="B2787" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2787" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2787" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2787" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2787" t="n">
+        <v>52</v>
+      </c>
+      <c r="G2787" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2787" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2787" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2788">
+      <c r="A2788" s="1" t="n">
+        <v>44005.4467915625</v>
+      </c>
+      <c r="B2788" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2788" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2788" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2788" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2788" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2788" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2788" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2788" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2789">
+      <c r="A2789" s="1" t="n">
+        <v>44005.4582543171</v>
+      </c>
+      <c r="B2789" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2789" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2789" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2789" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2789" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2789" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2789" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2789" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2790">
+      <c r="A2790" s="1" t="n">
+        <v>44005.4593176736</v>
+      </c>
+      <c r="B2790" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2790" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2790" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2790" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2790" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2790" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2790" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2790" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2791">
+      <c r="A2791" s="1" t="n">
+        <v>44005.474418588</v>
+      </c>
+      <c r="B2791" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2791" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2791" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2791" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2791" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2791" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2791" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2791" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2792">
+      <c r="A2792" s="1" t="n">
+        <v>44005.476614919</v>
+      </c>
+      <c r="B2792" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2792" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2792" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2792" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2792" t="n">
+        <v>72</v>
+      </c>
+      <c r="G2792" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2792" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2792" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2793">
+      <c r="A2793" s="1" t="n">
+        <v>44005.4787971065</v>
+      </c>
+      <c r="B2793" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2793" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2793" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2793" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2793" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2793" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2793" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2793" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2794">
+      <c r="A2794" s="1" t="n">
+        <v>44005.4838022106</v>
+      </c>
+      <c r="B2794" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2794" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2794" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2794" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2794" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2794" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2794" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2794" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2795">
+      <c r="A2795" s="1" t="n">
+        <v>44005.5014145255</v>
+      </c>
+      <c r="B2795" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2795" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2795" t="n">
+        <v>47</v>
+      </c>
+      <c r="E2795" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2795" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2795" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2795" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2795" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2796">
+      <c r="A2796" s="1" t="n">
+        <v>44005.5653323727</v>
+      </c>
+      <c r="B2796" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2796"/>
+      <c r="D2796" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2796" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2796" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2796" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2796" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2796" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2797">
+      <c r="A2797" s="1" t="n">
+        <v>44005.596984456</v>
+      </c>
+      <c r="B2797" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2797" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2797" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2797" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2797" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2797" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2797" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2797" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2798">
+      <c r="A2798" s="1" t="n">
+        <v>44005.6561149306</v>
+      </c>
+      <c r="B2798" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2798" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2798" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2798" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2798" t="n">
+        <v>46</v>
+      </c>
+      <c r="G2798" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2798" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2798" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2799">
+      <c r="A2799" s="1" t="n">
+        <v>44005.6630473032</v>
+      </c>
+      <c r="B2799" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2799" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2799" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2799" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2799" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2799" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2799" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2799" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2800">
+      <c r="A2800" s="1" t="n">
+        <v>44005.7331559259</v>
+      </c>
+      <c r="B2800" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2800" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2800" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2800" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2800" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2800" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2800" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2800" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2801">
+      <c r="A2801" s="1" t="n">
+        <v>44005.7706996528</v>
+      </c>
+      <c r="B2801" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2801" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2801" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2801" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2801" t="n">
+        <v>26</v>
+      </c>
+      <c r="G2801" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2801" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2801" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2802">
+      <c r="A2802" s="1" t="n">
+        <v>44005.8009845833</v>
+      </c>
+      <c r="B2802" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2802" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2802" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2802" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2802" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2802" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2802" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2802" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2803">
+      <c r="A2803" s="1" t="n">
+        <v>44005.8623163426</v>
+      </c>
+      <c r="B2803" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2803" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2803" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2803" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2803" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2803" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2803" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2803" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2804">
+      <c r="A2804" s="1" t="n">
+        <v>44006.0229105324</v>
+      </c>
+      <c r="B2804" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2804" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2804" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2804" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2804" t="n">
+        <v>65</v>
+      </c>
+      <c r="G2804" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2804" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2804" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2805">
+      <c r="A2805" s="1" t="n">
+        <v>44006.3286808449</v>
+      </c>
+      <c r="B2805" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2805" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2805" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2805" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2805" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2805" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2805" t="n">
+        <v>45</v>
+      </c>
+      <c r="I2805" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2806">
+      <c r="A2806" s="1" t="n">
+        <v>44006.3294286574</v>
+      </c>
+      <c r="B2806" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2806" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2806" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2806" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2806" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2806" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2806" t="n">
+        <v>42</v>
+      </c>
+      <c r="I2806" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2807">
+      <c r="A2807" s="1" t="n">
+        <v>44006.3535103935</v>
+      </c>
+      <c r="B2807" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2807" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2807" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2807" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2807" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2807" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2807" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2807" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2808">
+      <c r="A2808" s="1" t="n">
+        <v>44006.3633799074</v>
+      </c>
+      <c r="B2808" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2808" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2808" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2808" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2808" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2808" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2808" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2808" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2809">
+      <c r="A2809" s="1" t="n">
+        <v>44006.3654233681</v>
+      </c>
+      <c r="B2809" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2809" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2809" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2809" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2809" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2809" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2809" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2809" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2810">
+      <c r="A2810" s="1" t="n">
+        <v>44006.3698384143</v>
+      </c>
+      <c r="B2810" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2810" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2810" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2810" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2810" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2810" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2810" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2810" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2811">
+      <c r="A2811" s="1" t="n">
+        <v>44006.3753717593</v>
+      </c>
+      <c r="B2811" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2811" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2811" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2811" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2811" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2811" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2811" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2811" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2812">
+      <c r="A2812" s="1" t="n">
+        <v>44006.3760919792</v>
+      </c>
+      <c r="B2812" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2812" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2812" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2812" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2812" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2812" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2812" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2812" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2813">
+      <c r="A2813" s="1" t="n">
+        <v>44006.3878080208</v>
+      </c>
+      <c r="B2813" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2813" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2813" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2813" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2813" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2813" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2813" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2813" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2814">
+      <c r="A2814" s="1" t="n">
+        <v>44006.3938132523</v>
+      </c>
+      <c r="B2814" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2814" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2814" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2814" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2814" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2814" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2814" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2814" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2815">
+      <c r="A2815" s="1" t="n">
+        <v>44006.4037261805</v>
+      </c>
+      <c r="B2815" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2815" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2815" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2815" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2815" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2815" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2815" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2815" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Criação da função das previsões de datas de estouro dos leitos
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -421,6 +421,21 @@
   <si>
     <t xml:space="preserve">renatocvaz@hotmail.com</t>
   </si>
+  <si>
+    <t xml:space="preserve">ale_gaby@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instituto de Cardiologia - UTI PEDIATRICA - TIPO III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">janainahuber@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tzvi.voy@terra.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fnGel@hcpa.edu.br</t>
+  </si>
 </sst>
 </file>
 
@@ -82392,6 +82407,2471 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2816">
+      <c r="A2816" s="1" t="n">
+        <v>44006.4145049306</v>
+      </c>
+      <c r="B2816" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2816" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2816" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2816" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2816" t="n">
+        <v>49</v>
+      </c>
+      <c r="G2816" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2816" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2816" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2817">
+      <c r="A2817" s="1" t="n">
+        <v>44006.4191078009</v>
+      </c>
+      <c r="B2817" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2817" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2817" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2817" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2817" t="n">
+        <v>57</v>
+      </c>
+      <c r="G2817" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2817" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2817" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2818">
+      <c r="A2818" s="1" t="n">
+        <v>44006.4333765856</v>
+      </c>
+      <c r="B2818" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2818" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2818" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2818" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2818" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2818" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2818" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2818" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2819">
+      <c r="A2819" s="1" t="n">
+        <v>44006.4341651736</v>
+      </c>
+      <c r="B2819" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2819" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2819" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2819" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2819" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2819" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2819" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2819" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2820">
+      <c r="A2820" s="1" t="n">
+        <v>44006.4546553125</v>
+      </c>
+      <c r="B2820" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2820" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2820" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2820" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2820" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2820" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2820" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2820" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2821">
+      <c r="A2821" s="1" t="n">
+        <v>44006.476078206</v>
+      </c>
+      <c r="B2821" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2821" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2821" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2821" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2821" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2821" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2821" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2821" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2822">
+      <c r="A2822" s="1" t="n">
+        <v>44006.4824535069</v>
+      </c>
+      <c r="B2822" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2822" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2822" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2822" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2822" t="n">
+        <v>71</v>
+      </c>
+      <c r="G2822" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2822" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2822" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2823">
+      <c r="A2823" s="1" t="n">
+        <v>44006.4827156944</v>
+      </c>
+      <c r="B2823" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2823" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2823" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2823" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2823" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2823" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2823" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2823" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2824">
+      <c r="A2824" s="1" t="n">
+        <v>44006.4903342361</v>
+      </c>
+      <c r="B2824" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2824" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2824" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2824" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2824" t="n">
+        <v>47</v>
+      </c>
+      <c r="G2824" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2824" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2824" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2825">
+      <c r="A2825" s="1" t="n">
+        <v>44006.5374093634</v>
+      </c>
+      <c r="B2825" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2825" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2825" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2825" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2825" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2825" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2825" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2825" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2826">
+      <c r="A2826" s="1" t="n">
+        <v>44006.5504068634</v>
+      </c>
+      <c r="B2826" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2826" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2826" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2826" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2826" t="n">
+        <v>52</v>
+      </c>
+      <c r="G2826" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2826" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2826" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2827">
+      <c r="A2827" s="1" t="n">
+        <v>44006.5890965393</v>
+      </c>
+      <c r="B2827" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2827" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2827" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2827" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2827" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2827" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2827" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2827" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2828">
+      <c r="A2828" s="1" t="n">
+        <v>44006.6126827315</v>
+      </c>
+      <c r="B2828" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2828" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2828" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2828" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2828" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2828" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2828" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2828" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2829">
+      <c r="A2829" s="1" t="n">
+        <v>44006.6451861343</v>
+      </c>
+      <c r="B2829" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2829" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2829" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2829" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2829" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2829" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2829" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2829" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2830">
+      <c r="A2830" s="1" t="n">
+        <v>44006.7185063079</v>
+      </c>
+      <c r="B2830" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2830" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2830" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2830" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2830" t="n">
+        <v>38</v>
+      </c>
+      <c r="G2830" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2830" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2830" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2831">
+      <c r="A2831" s="1" t="n">
+        <v>44006.7267977546</v>
+      </c>
+      <c r="B2831" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2831" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2831" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2831" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2831" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2831" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2831" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2831" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2832">
+      <c r="A2832" s="1" t="n">
+        <v>44006.7459686921</v>
+      </c>
+      <c r="B2832" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2832" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2832" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2832" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2832" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2832" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2832" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2832" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2833">
+      <c r="A2833" s="1" t="n">
+        <v>44006.7912114699</v>
+      </c>
+      <c r="B2833" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2833" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2833" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2833" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2833" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2833" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2833" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2833" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2834">
+      <c r="A2834" s="1" t="n">
+        <v>44006.7971709375</v>
+      </c>
+      <c r="B2834" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2834" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2834" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2834" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2834" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2834" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2834" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2834" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2835">
+      <c r="A2835" s="1" t="n">
+        <v>44006.8291111343</v>
+      </c>
+      <c r="B2835" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2835" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2835" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2835" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2835" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2835" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2835" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2835" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2836">
+      <c r="A2836" s="1" t="n">
+        <v>44006.9599368055</v>
+      </c>
+      <c r="B2836" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2836" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2836" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2836" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2836" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2836" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2836" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2836" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2837">
+      <c r="A2837" s="1" t="n">
+        <v>44006.9603568287</v>
+      </c>
+      <c r="B2837" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2837" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2837" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2837" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2837" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2837" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2837" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2837" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2838">
+      <c r="A2838" s="1" t="n">
+        <v>44006.969244294</v>
+      </c>
+      <c r="B2838" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2838" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2838" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2838" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2838" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2838" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2838" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2838" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2839">
+      <c r="A2839" s="1" t="n">
+        <v>44007.286336331</v>
+      </c>
+      <c r="B2839" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2839" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2839" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2839" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2839" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2839" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2839" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2839" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2840">
+      <c r="A2840" s="1" t="n">
+        <v>44007.286626794</v>
+      </c>
+      <c r="B2840" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2840" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2840" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2840" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2840" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2840" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2840" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2840" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2841">
+      <c r="A2841" s="1" t="n">
+        <v>44007.3151358449</v>
+      </c>
+      <c r="B2841" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2841" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2841" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2841" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2841" t="n">
+        <v>96</v>
+      </c>
+      <c r="G2841" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2841" t="n">
+        <v>42</v>
+      </c>
+      <c r="I2841" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2842">
+      <c r="A2842" s="1" t="n">
+        <v>44007.3157901157</v>
+      </c>
+      <c r="B2842" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2842" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2842" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2842" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2842" t="n">
+        <v>101</v>
+      </c>
+      <c r="G2842" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2842" t="n">
+        <v>45</v>
+      </c>
+      <c r="I2842" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2843">
+      <c r="A2843" s="1" t="n">
+        <v>44007.3225504861</v>
+      </c>
+      <c r="B2843" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2843" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2843" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2843" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2843" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2843" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2843" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2843" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2844">
+      <c r="A2844" s="1" t="n">
+        <v>44007.3231790625</v>
+      </c>
+      <c r="B2844" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2844" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2844" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2844" t="n">
+        <v>9</v>
+      </c>
+      <c r="F2844" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2844" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2844" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2844" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2845">
+      <c r="A2845" s="1" t="n">
+        <v>44007.3346721643</v>
+      </c>
+      <c r="B2845" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2845" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2845" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2845" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2845" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2845" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2845" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2845" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2846">
+      <c r="A2846" s="1" t="n">
+        <v>44007.3378412384</v>
+      </c>
+      <c r="B2846" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2846" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2846" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2846" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2846" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2846" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2846" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2846" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2847">
+      <c r="A2847" s="1" t="n">
+        <v>44007.365153912</v>
+      </c>
+      <c r="B2847" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2847" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2847" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2847" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2847" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2847" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2847" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2847" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2848">
+      <c r="A2848" s="1" t="n">
+        <v>44007.3673885648</v>
+      </c>
+      <c r="B2848" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2848" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2848" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2848" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2848" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2848" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2848" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2848" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2849">
+      <c r="A2849" s="1" t="n">
+        <v>44007.3868412616</v>
+      </c>
+      <c r="B2849" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2849" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2849" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2849" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2849" t="n">
+        <v>12</v>
+      </c>
+      <c r="G2849" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2849" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2849" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2850">
+      <c r="A2850" s="1" t="n">
+        <v>44007.4055994329</v>
+      </c>
+      <c r="B2850" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2850" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2850" t="n">
+        <v>69</v>
+      </c>
+      <c r="E2850" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2850" t="n">
+        <v>55</v>
+      </c>
+      <c r="G2850" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2850" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2850" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2851">
+      <c r="A2851" s="1" t="n">
+        <v>44007.4071135648</v>
+      </c>
+      <c r="B2851" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2851" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2851" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2851" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2851" t="n">
+        <v>58</v>
+      </c>
+      <c r="G2851" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2851" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2851" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2852">
+      <c r="A2852" s="1" t="n">
+        <v>44007.4080055787</v>
+      </c>
+      <c r="B2852" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2852" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2852" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2852" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2852" t="n">
+        <v>58</v>
+      </c>
+      <c r="G2852" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2852" t="n">
+        <v>58</v>
+      </c>
+      <c r="I2852" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2853">
+      <c r="A2853" s="1" t="n">
+        <v>44007.4083214583</v>
+      </c>
+      <c r="B2853" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2853" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2853" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2853" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2853" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2853" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2853" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2853" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2854">
+      <c r="A2854" s="1" t="n">
+        <v>44007.4132295023</v>
+      </c>
+      <c r="B2854" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2854" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2854" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2854" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2854" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2854" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2854" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2854" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2855">
+      <c r="A2855" s="1" t="n">
+        <v>44007.418166794</v>
+      </c>
+      <c r="B2855" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2855" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2855" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2855" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2855" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2855" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2855" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2855" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2856">
+      <c r="A2856" s="1" t="n">
+        <v>44007.4212117014</v>
+      </c>
+      <c r="B2856" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2856" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2856" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2856" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2856" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2856" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2856" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2856" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2857">
+      <c r="A2857" s="1" t="n">
+        <v>44007.422833588</v>
+      </c>
+      <c r="B2857" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2857" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2857" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2857" t="n">
+        <v>15</v>
+      </c>
+      <c r="F2857" t="n">
+        <v>54</v>
+      </c>
+      <c r="G2857" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2857" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2857" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2858">
+      <c r="A2858" s="1" t="n">
+        <v>44007.4268163889</v>
+      </c>
+      <c r="B2858" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2858" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2858" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2858" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2858" t="n">
+        <v>41</v>
+      </c>
+      <c r="G2858" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2858" t="n">
+        <v>13</v>
+      </c>
+      <c r="I2858" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2859">
+      <c r="A2859" s="1" t="n">
+        <v>44007.4323383102</v>
+      </c>
+      <c r="B2859" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2859" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2859" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2859" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2859" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2859" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2859" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2859" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2860">
+      <c r="A2860" s="1" t="n">
+        <v>44007.4557555093</v>
+      </c>
+      <c r="B2860" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2860" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2860" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2860" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2860" t="n">
+        <v>58</v>
+      </c>
+      <c r="G2860" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2860" t="n">
+        <v>58</v>
+      </c>
+      <c r="I2860" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2861">
+      <c r="A2861" s="1" t="n">
+        <v>44007.4648160069</v>
+      </c>
+      <c r="B2861" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2861" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2861" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2861" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2861" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2861" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2861" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2861" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2862">
+      <c r="A2862" s="1" t="n">
+        <v>44007.4653004977</v>
+      </c>
+      <c r="B2862" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2862" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2862" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2862" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2862" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2862" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2862" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2862" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2863">
+      <c r="A2863" s="1" t="n">
+        <v>44007.4735204745</v>
+      </c>
+      <c r="B2863" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2863" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2863" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2863" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2863" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2863" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2863" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2863" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2864">
+      <c r="A2864" s="1" t="n">
+        <v>44007.4761518518</v>
+      </c>
+      <c r="B2864" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2864" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2864" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2864" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2864" t="n">
+        <v>57</v>
+      </c>
+      <c r="G2864" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2864" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2864" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2865">
+      <c r="A2865" s="1" t="n">
+        <v>44007.4762466551</v>
+      </c>
+      <c r="B2865" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2865" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2865" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2865" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2865" t="n">
+        <v>57</v>
+      </c>
+      <c r="G2865" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2865" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2865" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2866">
+      <c r="A2866" s="1" t="n">
+        <v>44007.4766362384</v>
+      </c>
+      <c r="B2866" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2866" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2866" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2866" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2866" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2866" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2866" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2866" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2867">
+      <c r="A2867" s="1" t="n">
+        <v>44007.4772197801</v>
+      </c>
+      <c r="B2867" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2867" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2867" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2867" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2867" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2867" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2867" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2867" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2868">
+      <c r="A2868" s="1" t="n">
+        <v>44007.4774160417</v>
+      </c>
+      <c r="B2868" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2868" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2868" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2868" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2868" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2868" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2868" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2868" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2869">
+      <c r="A2869" s="1" t="n">
+        <v>44007.4780662153</v>
+      </c>
+      <c r="B2869" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2869" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2869" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2869" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2869" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2869" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2869" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2869" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2870">
+      <c r="A2870" s="1" t="n">
+        <v>44007.4867321065</v>
+      </c>
+      <c r="B2870" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2870" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2870" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2870" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2870" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2870" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2870" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2870" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2871">
+      <c r="A2871" s="1" t="n">
+        <v>44007.4951979745</v>
+      </c>
+      <c r="B2871" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2871" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2871" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2871" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2871" t="n">
+        <v>68</v>
+      </c>
+      <c r="G2871" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2871" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2871" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2872">
+      <c r="A2872" s="1" t="n">
+        <v>44007.4956093981</v>
+      </c>
+      <c r="B2872" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2872" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2872" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2872" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2872" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2872" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2872" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2872" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2873">
+      <c r="A2873" s="1" t="n">
+        <v>44007.5337861574</v>
+      </c>
+      <c r="B2873" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2873" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2873" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2873" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2873" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2873" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2873" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2873" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2874">
+      <c r="A2874" s="1" t="n">
+        <v>44007.5496118634</v>
+      </c>
+      <c r="B2874" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2874" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2874" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2874" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2874" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2874" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2874" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2874" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2875">
+      <c r="A2875" s="1" t="n">
+        <v>44007.5809525347</v>
+      </c>
+      <c r="B2875" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2875" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2875" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2875" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2875" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2875" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2875" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2875" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2876">
+      <c r="A2876" s="1" t="n">
+        <v>44007.7929064931</v>
+      </c>
+      <c r="B2876" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2876" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2876" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2876" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2876" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2876" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2876" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2876" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2877">
+      <c r="A2877" s="1" t="n">
+        <v>44007.8242628588</v>
+      </c>
+      <c r="B2877" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2877" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2877" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2877" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2877" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2877" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2877" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2877" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2878">
+      <c r="A2878" s="1" t="n">
+        <v>44007.9886700231</v>
+      </c>
+      <c r="B2878" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2878" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2878" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2878" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2878" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2878" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2878" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2878" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2879">
+      <c r="A2879" s="1" t="n">
+        <v>44008.2684977431</v>
+      </c>
+      <c r="B2879" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2879" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2879" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2879" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2879" t="n">
+        <v>101</v>
+      </c>
+      <c r="G2879" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2879" t="n">
+        <v>45</v>
+      </c>
+      <c r="I2879" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2880">
+      <c r="A2880" s="1" t="n">
+        <v>44008.2691522685</v>
+      </c>
+      <c r="B2880" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2880" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2880" t="n">
+        <v>128</v>
+      </c>
+      <c r="E2880" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2880" t="n">
+        <v>98</v>
+      </c>
+      <c r="G2880" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2880" t="n">
+        <v>47</v>
+      </c>
+      <c r="I2880" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2881">
+      <c r="A2881" s="1" t="n">
+        <v>44008.3228744792</v>
+      </c>
+      <c r="B2881" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2881" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2881" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2881" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2881" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2881" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2881" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2881" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2882">
+      <c r="A2882" s="1" t="n">
+        <v>44008.3279780208</v>
+      </c>
+      <c r="B2882" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2882" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2882" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2882" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2882" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2882" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2882" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2882" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2883">
+      <c r="A2883" s="1" t="n">
+        <v>44008.3375210069</v>
+      </c>
+      <c r="B2883" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2883" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2883" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2883" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2883" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2883" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2883" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2883" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2884">
+      <c r="A2884" s="1" t="n">
+        <v>44008.3644681366</v>
+      </c>
+      <c r="B2884" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2884" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2884" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2884" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2884" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2884" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2884" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2884" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2885">
+      <c r="A2885" s="1" t="n">
+        <v>44008.3925070486</v>
+      </c>
+      <c r="B2885" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2885" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2885" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2885" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2885" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2885" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2885" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2885" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2886">
+      <c r="A2886" s="1" t="n">
+        <v>44008.4028619444</v>
+      </c>
+      <c r="B2886" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2886" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2886" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2886" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2886" t="n">
+        <v>27</v>
+      </c>
+      <c r="G2886" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2886" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2886" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2887">
+      <c r="A2887" s="1" t="n">
+        <v>44008.4048978935</v>
+      </c>
+      <c r="B2887" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2887" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2887" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2887" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2887" t="n">
+        <v>56</v>
+      </c>
+      <c r="G2887" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2887" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2887" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2888">
+      <c r="A2888" s="1" t="n">
+        <v>44008.4066557639</v>
+      </c>
+      <c r="B2888" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2888" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2888" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2888" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2888" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2888" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2888" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2888" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2889">
+      <c r="A2889" s="1" t="n">
+        <v>44008.4088800926</v>
+      </c>
+      <c r="B2889" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2889" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2889" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2889" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2889" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2889" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2889" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2889" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2890">
+      <c r="A2890" s="1" t="n">
+        <v>44008.4248471528</v>
+      </c>
+      <c r="B2890" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2890" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2890" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2890" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2890" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2890" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2890" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2890" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2891">
+      <c r="A2891" s="1" t="n">
+        <v>44008.4261176273</v>
+      </c>
+      <c r="B2891" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2891" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2891" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2891" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2891" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2891" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2891" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2891" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2892">
+      <c r="A2892" s="1" t="n">
+        <v>44008.443271713</v>
+      </c>
+      <c r="B2892" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2892" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2892" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2892" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2892" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2892" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2892" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2892" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2893">
+      <c r="A2893" s="1" t="n">
+        <v>44008.4477044676</v>
+      </c>
+      <c r="B2893" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2893" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2893" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2893" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2893" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2893" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2893" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2893" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2894">
+      <c r="A2894" s="1" t="n">
+        <v>44008.4567974769</v>
+      </c>
+      <c r="B2894" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2894" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2894" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2894" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2894" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2894" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2894" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2894" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2895">
+      <c r="A2895" s="1" t="n">
+        <v>44008.4831045718</v>
+      </c>
+      <c r="B2895" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2895" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2895" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2895" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2895" t="n">
+        <v>52</v>
+      </c>
+      <c r="G2895" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2895" t="n">
+        <v>13</v>
+      </c>
+      <c r="I2895" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2896">
+      <c r="A2896" s="1" t="n">
+        <v>44008.50021625</v>
+      </c>
+      <c r="B2896" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2896" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2896" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2896" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2896" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2896" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2896" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2896" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2897">
+      <c r="A2897" s="1" t="n">
+        <v>44008.532814838</v>
+      </c>
+      <c r="B2897" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2897" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2897" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2897" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2897" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2897" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2897" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2897" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2898">
+      <c r="A2898" s="1" t="n">
+        <v>44008.5341776042</v>
+      </c>
+      <c r="B2898" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2898" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2898" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2898" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2898" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2898" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2898" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2898" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2899">
+      <c r="A2899" s="1" t="n">
+        <v>44008.5457758102</v>
+      </c>
+      <c r="B2899" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2899" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2899" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2899" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2899" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2899" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2899" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2899" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2900">
+      <c r="A2900" s="1" t="n">
+        <v>44008.562637037</v>
+      </c>
+      <c r="B2900" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2900" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2900" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2900" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2900" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2900" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2900" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2900" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
inclusão das previsões do estouro de leitos Inclusão da média de pacientes por dia na regressão
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -436,6 +436,21 @@
   <si>
     <t xml:space="preserve">fnGel@hcpa.edu.br</t>
   </si>
+  <si>
+    <t xml:space="preserve">analise.medina@divinaprovidencia.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tzvivoy@terra.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fernanda.ms@santacasa.tche.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roiter.furtado@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taivrg@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -81836,7 +81851,9 @@
       <c r="B2796" t="s">
         <v>83</v>
       </c>
-      <c r="C2796"/>
+      <c r="C2796" t="s">
+        <v>38</v>
+      </c>
       <c r="D2796" t="n">
         <v>18</v>
       </c>
@@ -84869,6 +84886,3511 @@
         <v>1</v>
       </c>
       <c r="I2900" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2901">
+      <c r="A2901" s="1" t="n">
+        <v>44008.5908130903</v>
+      </c>
+      <c r="B2901" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2901" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2901" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2901" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2901" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2901" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2901" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2901" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2902">
+      <c r="A2902" s="1" t="n">
+        <v>44008.5989559607</v>
+      </c>
+      <c r="B2902" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2902" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2902" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2902" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2902" t="n">
+        <v>64</v>
+      </c>
+      <c r="G2902" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2902" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2902" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2903">
+      <c r="A2903" s="1" t="n">
+        <v>44008.6000406597</v>
+      </c>
+      <c r="B2903" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2903" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2903" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2903" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2903" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2903" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2903" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2903" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2904">
+      <c r="A2904" s="1" t="n">
+        <v>44008.6228558912</v>
+      </c>
+      <c r="B2904" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2904" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2904" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2904" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2904" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2904" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2904" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2904" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2905">
+      <c r="A2905" s="1" t="n">
+        <v>44008.6461491204</v>
+      </c>
+      <c r="B2905" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2905" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2905" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2905" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2905" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2905" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2905" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2905" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2906">
+      <c r="A2906" s="1" t="n">
+        <v>44008.6825808218</v>
+      </c>
+      <c r="B2906" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2906" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2906" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2906" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2906" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2906" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2906" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2906" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2907">
+      <c r="A2907" s="1" t="n">
+        <v>44008.6916074884</v>
+      </c>
+      <c r="B2907" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2907" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2907" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2907" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2907" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2907" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2907" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2907" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2908">
+      <c r="A2908" s="1" t="n">
+        <v>44008.7205090509</v>
+      </c>
+      <c r="B2908" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2908" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2908" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2908" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2908" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2908" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2908" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2908" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2909">
+      <c r="A2909" s="1" t="n">
+        <v>44008.7207111227</v>
+      </c>
+      <c r="B2909" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2909" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2909" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2909" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2909" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2909" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2909" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2909" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2910">
+      <c r="A2910" s="1" t="n">
+        <v>44008.766724375</v>
+      </c>
+      <c r="B2910" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2910"/>
+      <c r="D2910" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2910" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2910" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2910" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2910" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2910" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2911">
+      <c r="A2911" s="1" t="n">
+        <v>44008.7670501505</v>
+      </c>
+      <c r="B2911" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2911" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2911" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2911" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2911" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2911" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2911" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2911" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2912">
+      <c r="A2912" s="1" t="n">
+        <v>44008.7943500694</v>
+      </c>
+      <c r="B2912" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2912" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2912" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2912" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2912" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2912" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2912" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2912" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2913">
+      <c r="A2913" s="1" t="n">
+        <v>44008.8344226505</v>
+      </c>
+      <c r="B2913" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2913" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2913" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2913" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2913" t="n">
+        <v>16</v>
+      </c>
+      <c r="G2913" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2913" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2913" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2914">
+      <c r="A2914" s="1" t="n">
+        <v>44008.8353292245</v>
+      </c>
+      <c r="B2914" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2914" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2914" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2914" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2914" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2914" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2914" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2914" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2915">
+      <c r="A2915" s="1" t="n">
+        <v>44008.8416551042</v>
+      </c>
+      <c r="B2915" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2915" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2915" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2915" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2915" t="n">
+        <v>56</v>
+      </c>
+      <c r="G2915" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2915" t="n">
+        <v>26</v>
+      </c>
+      <c r="I2915" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2916">
+      <c r="A2916" s="1" t="n">
+        <v>44008.8426137616</v>
+      </c>
+      <c r="B2916" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2916" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2916" t="n">
+        <v>69</v>
+      </c>
+      <c r="E2916" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2916" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2916" t="n">
+        <v>14</v>
+      </c>
+      <c r="H2916" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2916" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2917">
+      <c r="A2917" s="1" t="n">
+        <v>44008.8988933449</v>
+      </c>
+      <c r="B2917" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2917" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2917" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2917" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2917" t="n">
+        <v>55</v>
+      </c>
+      <c r="G2917" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2917" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2917" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2918">
+      <c r="A2918" s="1" t="n">
+        <v>44009.3164502199</v>
+      </c>
+      <c r="B2918" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2918" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2918" t="n">
+        <v>60</v>
+      </c>
+      <c r="E2918" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2918" t="n">
+        <v>42</v>
+      </c>
+      <c r="G2918" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2918" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2918" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2919">
+      <c r="A2919" s="1" t="n">
+        <v>44009.3450690278</v>
+      </c>
+      <c r="B2919" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2919" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2919" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2919" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2919" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2919" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2919" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2919" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2920">
+      <c r="A2920" s="1" t="n">
+        <v>44009.3723936227</v>
+      </c>
+      <c r="B2920" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2920" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2920" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2920" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2920" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2920" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2920" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2920" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2921">
+      <c r="A2921" s="1" t="n">
+        <v>44009.3760201389</v>
+      </c>
+      <c r="B2921" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2921" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2921" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2921" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2921" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2921" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2921" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2921" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2922">
+      <c r="A2922" s="1" t="n">
+        <v>44009.3764510185</v>
+      </c>
+      <c r="B2922" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2922" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2922" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2922" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2922" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2922" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2922" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2922" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2923">
+      <c r="A2923" s="1" t="n">
+        <v>44009.3780357755</v>
+      </c>
+      <c r="B2923" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2923" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2923" t="n">
+        <v>133</v>
+      </c>
+      <c r="E2923" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2923" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2923" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2923" t="n">
+        <v>49</v>
+      </c>
+      <c r="I2923" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2924">
+      <c r="A2924" s="1" t="n">
+        <v>44009.3880351505</v>
+      </c>
+      <c r="B2924" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2924" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2924" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2924" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2924" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2924" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2924" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2924" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2925">
+      <c r="A2925" s="1" t="n">
+        <v>44009.4153133102</v>
+      </c>
+      <c r="B2925" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2925" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2925" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2925" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2925" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2925" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2925" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2925" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2926">
+      <c r="A2926" s="1" t="n">
+        <v>44009.4282501389</v>
+      </c>
+      <c r="B2926" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2926" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2926" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2926" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2926" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2926" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2926" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2926" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2927">
+      <c r="A2927" s="1" t="n">
+        <v>44009.4339308333</v>
+      </c>
+      <c r="B2927" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2927" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2927" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2927" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2927" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2927" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2927" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2927" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2928">
+      <c r="A2928" s="1" t="n">
+        <v>44009.4366156134</v>
+      </c>
+      <c r="B2928" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2928" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2928" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2928" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2928" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2928" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2928" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2928" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2929">
+      <c r="A2929" s="1" t="n">
+        <v>44009.4453892245</v>
+      </c>
+      <c r="B2929" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2929" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2929" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2929" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2929" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2929" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2929" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2929" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2930">
+      <c r="A2930" s="1" t="n">
+        <v>44009.4590645255</v>
+      </c>
+      <c r="B2930" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2930" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2930" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2930" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2930" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2930" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2930" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2930" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2931">
+      <c r="A2931" s="1" t="n">
+        <v>44009.4776198495</v>
+      </c>
+      <c r="B2931" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2931" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2931" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2931" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2931" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2931" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2931" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2931" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2932">
+      <c r="A2932" s="1" t="n">
+        <v>44009.488073912</v>
+      </c>
+      <c r="B2932" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2932" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2932" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2932" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2932" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2932" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2932" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2932" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2933">
+      <c r="A2933" s="1" t="n">
+        <v>44009.4946643866</v>
+      </c>
+      <c r="B2933" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2933" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2933" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2933" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2933" t="n">
+        <v>64</v>
+      </c>
+      <c r="G2933" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2933" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2933" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2934">
+      <c r="A2934" s="1" t="n">
+        <v>44009.4958139931</v>
+      </c>
+      <c r="B2934" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2934" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2934" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2934" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2934" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2934" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2934" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2934" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2935">
+      <c r="A2935" s="1" t="n">
+        <v>44009.5327018634</v>
+      </c>
+      <c r="B2935" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2935" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2935" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2935" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2935" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2935" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2935" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2935" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2936">
+      <c r="A2936" s="1" t="n">
+        <v>44009.5550179745</v>
+      </c>
+      <c r="B2936" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2936" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2936" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2936" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2936" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2936" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2936" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2936" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2937">
+      <c r="A2937" s="1" t="n">
+        <v>44009.555648588</v>
+      </c>
+      <c r="B2937" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2937" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2937" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2937" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2937" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2937" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2937" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2937" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2938">
+      <c r="A2938" s="1" t="n">
+        <v>44009.5650480208</v>
+      </c>
+      <c r="B2938" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2938" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2938" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2938" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2938" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2938" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2938" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2938" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2939">
+      <c r="A2939" s="1" t="n">
+        <v>44009.5669429398</v>
+      </c>
+      <c r="B2939" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2939" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2939" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2939" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2939" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2939" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2939" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2939" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2940">
+      <c r="A2940" s="1" t="n">
+        <v>44009.6525607755</v>
+      </c>
+      <c r="B2940" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2940" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2940" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2940" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2940" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2940" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2940" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2940" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" s="1" t="n">
+        <v>44009.7370962153</v>
+      </c>
+      <c r="B2941" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2941" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2941" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2941" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2941" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2941" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2941" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2941" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" s="1" t="n">
+        <v>44009.7384631829</v>
+      </c>
+      <c r="B2942" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2942" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2942" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2942" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2942" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2942" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2942" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2942" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" s="1" t="n">
+        <v>44009.7780197685</v>
+      </c>
+      <c r="B2943" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2943" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2943" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2943" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2943" t="n">
+        <v>34</v>
+      </c>
+      <c r="G2943" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2943" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2943" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" s="1" t="n">
+        <v>44009.8136723495</v>
+      </c>
+      <c r="B2944" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2944" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2944" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2944" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2944" t="n">
+        <v>41</v>
+      </c>
+      <c r="G2944" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2944" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2944" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" s="1" t="n">
+        <v>44010.3488857176</v>
+      </c>
+      <c r="B2945" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2945" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2945" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2945" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2945" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2945" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2945" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2945" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" s="1" t="n">
+        <v>44010.3832576042</v>
+      </c>
+      <c r="B2946" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2946" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2946" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2946" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2946" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2946" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2946" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2946" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" s="1" t="n">
+        <v>44010.3907702315</v>
+      </c>
+      <c r="B2947" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2947" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2947" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2947" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2947" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2947" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2947" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2947" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" s="1" t="n">
+        <v>44010.3963789352</v>
+      </c>
+      <c r="B2948" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2948" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2948" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2948" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2948" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2948" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2948" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2948" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" s="1" t="n">
+        <v>44010.3963963657</v>
+      </c>
+      <c r="B2949" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2949" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2949" t="n">
+        <v>133</v>
+      </c>
+      <c r="E2949" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2949" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2949" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2949" t="n">
+        <v>49</v>
+      </c>
+      <c r="I2949" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" s="1" t="n">
+        <v>44010.396903588</v>
+      </c>
+      <c r="B2950" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2950" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2950" t="n">
+        <v>133</v>
+      </c>
+      <c r="E2950" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2950" t="n">
+        <v>106</v>
+      </c>
+      <c r="G2950" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2950" t="n">
+        <v>52</v>
+      </c>
+      <c r="I2950" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" s="1" t="n">
+        <v>44010.4001021181</v>
+      </c>
+      <c r="B2951" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2951" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2951" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2951" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2951" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2951" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2951" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2951" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" s="1" t="n">
+        <v>44010.4062504861</v>
+      </c>
+      <c r="B2952" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2952" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2952" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2952" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2952" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2952" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2952" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2952" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2953">
+      <c r="A2953" s="1" t="n">
+        <v>44010.4072583681</v>
+      </c>
+      <c r="B2953" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2953" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2953" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2953" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2953" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2953" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2953" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2953" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2954">
+      <c r="A2954" s="1" t="n">
+        <v>44010.4107196643</v>
+      </c>
+      <c r="B2954" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2954" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2954" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2954" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2954" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2954" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2954" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2954" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2955">
+      <c r="A2955" s="1" t="n">
+        <v>44010.4566477894</v>
+      </c>
+      <c r="B2955" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2955" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2955" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2955" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2955" t="n">
+        <v>28</v>
+      </c>
+      <c r="G2955" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2955" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2955" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2956">
+      <c r="A2956" s="1" t="n">
+        <v>44010.4603889815</v>
+      </c>
+      <c r="B2956" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2956" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2956" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2956" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2956" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2956" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2956" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2956" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2957">
+      <c r="A2957" s="1" t="n">
+        <v>44010.4605438773</v>
+      </c>
+      <c r="B2957" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2957" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2957" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2957" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2957" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2957" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2957" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2957" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2958">
+      <c r="A2958" s="1" t="n">
+        <v>44010.4657548495</v>
+      </c>
+      <c r="B2958" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2958" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2958" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2958" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2958" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2958" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2958" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2958" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2959">
+      <c r="A2959" s="1" t="n">
+        <v>44010.486648831</v>
+      </c>
+      <c r="B2959" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2959" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2959" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2959" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2959" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2959" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2959" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2959" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2960">
+      <c r="A2960" s="1" t="n">
+        <v>44010.4874007523</v>
+      </c>
+      <c r="B2960" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2960" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2960" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2960" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2960" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2960" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2960" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2960" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2961">
+      <c r="A2961" s="1" t="n">
+        <v>44010.498071007</v>
+      </c>
+      <c r="B2961" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2961" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2961" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2961" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2961" t="n">
+        <v>61</v>
+      </c>
+      <c r="G2961" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2961" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2961" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2962">
+      <c r="A2962" s="1" t="n">
+        <v>44010.499037963</v>
+      </c>
+      <c r="B2962" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2962" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2962" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2962" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2962" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2962" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2962" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2962" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2963">
+      <c r="A2963" s="1" t="n">
+        <v>44010.5024283102</v>
+      </c>
+      <c r="B2963" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2963" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2963" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2963" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2963" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2963" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2963" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2963" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2964">
+      <c r="A2964" s="1" t="n">
+        <v>44010.5424908796</v>
+      </c>
+      <c r="B2964" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2964" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2964" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2964" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2964" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2964" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2964" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2964" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2965">
+      <c r="A2965" s="1" t="n">
+        <v>44010.5695314931</v>
+      </c>
+      <c r="B2965" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2965" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2965" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2965" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2965" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2965" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2965" t="n">
+        <v>13</v>
+      </c>
+      <c r="I2965" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2966">
+      <c r="A2966" s="1" t="n">
+        <v>44010.5711520139</v>
+      </c>
+      <c r="B2966" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2966" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2966" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2966" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2966" t="n">
+        <v>45</v>
+      </c>
+      <c r="G2966" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2966" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2966" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2967">
+      <c r="A2967" s="1" t="n">
+        <v>44010.587070706</v>
+      </c>
+      <c r="B2967" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2967" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2967" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2967" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2967" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2967" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2967" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2967" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2968">
+      <c r="A2968" s="1" t="n">
+        <v>44010.5931112037</v>
+      </c>
+      <c r="B2968" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2968" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2968" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2968" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2968" t="n">
+        <v>14</v>
+      </c>
+      <c r="G2968" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2968" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2968" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2969">
+      <c r="A2969" s="1" t="n">
+        <v>44010.6074650347</v>
+      </c>
+      <c r="B2969" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2969" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2969" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2969" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2969" t="n">
+        <v>62</v>
+      </c>
+      <c r="G2969" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2969" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2969" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2970">
+      <c r="A2970" s="1" t="n">
+        <v>44010.7089941204</v>
+      </c>
+      <c r="B2970" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2970" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2970" t="n">
+        <v>101</v>
+      </c>
+      <c r="E2970" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2970" t="n">
+        <v>61</v>
+      </c>
+      <c r="G2970" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2970" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2970" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2971">
+      <c r="A2971" s="1" t="n">
+        <v>44010.7143754282</v>
+      </c>
+      <c r="B2971" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2971" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2971" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2971" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2971" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2971" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2971" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2971" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2972">
+      <c r="A2972" s="1" t="n">
+        <v>44011.3256429861</v>
+      </c>
+      <c r="B2972" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2972" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2972" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2972" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2972" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2972" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2972" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2972" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2973">
+      <c r="A2973" s="1" t="n">
+        <v>44011.3350515509</v>
+      </c>
+      <c r="B2973" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2973" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2973" t="n">
+        <v>13</v>
+      </c>
+      <c r="E2973" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2973" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2973" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2973" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2973" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2974">
+      <c r="A2974" s="1" t="n">
+        <v>44011.3473268634</v>
+      </c>
+      <c r="B2974" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2974" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2974" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2974" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2974" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2974" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2974" t="n">
+        <v>13</v>
+      </c>
+      <c r="I2974" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2975">
+      <c r="A2975" s="1" t="n">
+        <v>44011.3483120602</v>
+      </c>
+      <c r="B2975" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2975" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2975" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2975" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2975" t="n">
+        <v>35</v>
+      </c>
+      <c r="G2975" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2975" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2975" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2976">
+      <c r="A2976" s="1" t="n">
+        <v>44011.3529183218</v>
+      </c>
+      <c r="B2976" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2976" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2976" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2976" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2976" t="n">
+        <v>16</v>
+      </c>
+      <c r="G2976" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2976" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2976" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2977">
+      <c r="A2977" s="1" t="n">
+        <v>44011.3765663889</v>
+      </c>
+      <c r="B2977" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2977" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2977" t="n">
+        <v>56</v>
+      </c>
+      <c r="E2977" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2977" t="n">
+        <v>53</v>
+      </c>
+      <c r="G2977" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2977" t="n">
+        <v>14</v>
+      </c>
+      <c r="I2977" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2978">
+      <c r="A2978" s="1" t="n">
+        <v>44011.3843153356</v>
+      </c>
+      <c r="B2978" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2978" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2978" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2978" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2978" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2978" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2978" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2978" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2979">
+      <c r="A2979" s="1" t="n">
+        <v>44011.3965309491</v>
+      </c>
+      <c r="B2979" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2979"/>
+      <c r="D2979" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2979" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2979" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2979" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2979" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2979" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2980">
+      <c r="A2980" s="1" t="n">
+        <v>44011.3966129398</v>
+      </c>
+      <c r="B2980" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2980" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2980" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2980" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2980" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2980" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2980" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2980" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2981">
+      <c r="A2981" s="1" t="n">
+        <v>44011.3982684838</v>
+      </c>
+      <c r="B2981" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2981" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2981" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2981" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2981" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2981" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2981" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2981" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2982">
+      <c r="A2982" s="1" t="n">
+        <v>44011.3989686806</v>
+      </c>
+      <c r="B2982" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2982" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2982" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2982" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2982" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2982" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2982" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2982" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2983">
+      <c r="A2983" s="1" t="n">
+        <v>44011.4059666898</v>
+      </c>
+      <c r="B2983" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2983" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2983" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2983" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2983" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2983" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2983" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2983" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2984">
+      <c r="A2984" s="1" t="n">
+        <v>44011.4176500694</v>
+      </c>
+      <c r="B2984" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2984" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2984" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2984" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2984" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2984" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2984" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2984" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2985">
+      <c r="A2985" s="1" t="n">
+        <v>44011.4192267477</v>
+      </c>
+      <c r="B2985" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2985" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2985" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2985" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2985" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2985" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2985" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2985" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2986">
+      <c r="A2986" s="1" t="n">
+        <v>44011.4225272338</v>
+      </c>
+      <c r="B2986" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2986" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2986" t="n">
+        <v>55</v>
+      </c>
+      <c r="E2986" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2986" t="n">
+        <v>44</v>
+      </c>
+      <c r="G2986" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2986" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2986" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2987">
+      <c r="A2987" s="1" t="n">
+        <v>44011.4344278935</v>
+      </c>
+      <c r="B2987" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2987" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2987" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2987" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2987" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2987" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2987" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2987" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2988">
+      <c r="A2988" s="1" t="n">
+        <v>44011.4530994444</v>
+      </c>
+      <c r="B2988" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2988" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2988" t="n">
+        <v>75</v>
+      </c>
+      <c r="E2988" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2988" t="n">
+        <v>65</v>
+      </c>
+      <c r="G2988" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2988" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2988" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2989">
+      <c r="A2989" s="1" t="n">
+        <v>44011.4593573495</v>
+      </c>
+      <c r="B2989" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2989" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2989" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2989" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2989" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2989" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2989" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2989" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2990">
+      <c r="A2990" s="1" t="n">
+        <v>44011.4630568287</v>
+      </c>
+      <c r="B2990" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2990" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2990" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2990" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2990" t="n">
+        <v>37</v>
+      </c>
+      <c r="G2990" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2990" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2990" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2991">
+      <c r="A2991" s="1" t="n">
+        <v>44011.4666418171</v>
+      </c>
+      <c r="B2991" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2991" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2991" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2991" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2991" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2991" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2991" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2991" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2992">
+      <c r="A2992" s="1" t="n">
+        <v>44011.4736080671</v>
+      </c>
+      <c r="B2992" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2992" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2992" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2992" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2992" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2992" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2992" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2992" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2993">
+      <c r="A2993" s="1" t="n">
+        <v>44011.4874580671</v>
+      </c>
+      <c r="B2993" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2993" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2993" t="n">
+        <v>101</v>
+      </c>
+      <c r="E2993" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2993" t="n">
+        <v>61</v>
+      </c>
+      <c r="G2993" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2993" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2993" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2994">
+      <c r="A2994" s="1" t="n">
+        <v>44011.488971331</v>
+      </c>
+      <c r="B2994" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2994" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2994" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2994" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2994" t="n">
+        <v>29</v>
+      </c>
+      <c r="G2994" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2994" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2994" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2995">
+      <c r="A2995" s="1" t="n">
+        <v>44011.502064618</v>
+      </c>
+      <c r="B2995" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2995" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2995" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2995" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2995" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2995" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2995" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2995" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2996">
+      <c r="A2996" s="1" t="n">
+        <v>44011.5025856944</v>
+      </c>
+      <c r="B2996" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2996" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2996" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2996" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2996" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2996" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2996" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2996" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2997">
+      <c r="A2997" s="1" t="n">
+        <v>44011.5295411574</v>
+      </c>
+      <c r="B2997" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2997" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2997" t="n">
+        <v>48</v>
+      </c>
+      <c r="E2997" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2997" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2997" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2997" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2997" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2998">
+      <c r="A2998" s="1" t="n">
+        <v>44011.598862662</v>
+      </c>
+      <c r="B2998" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2998" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2998" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2998" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2998" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2998" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2998" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2998" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2999">
+      <c r="A2999" s="1" t="n">
+        <v>44011.7124446644</v>
+      </c>
+      <c r="B2999" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2999" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2999" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2999" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2999" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2999" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2999" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2999" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3000">
+      <c r="A3000" s="1" t="n">
+        <v>44011.7472756944</v>
+      </c>
+      <c r="B3000" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3000" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3000" t="n">
+        <v>133</v>
+      </c>
+      <c r="E3000" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3000" t="n">
+        <v>106</v>
+      </c>
+      <c r="G3000" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3000" t="n">
+        <v>52</v>
+      </c>
+      <c r="I3000" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3001">
+      <c r="A3001" s="1" t="n">
+        <v>44011.747938125</v>
+      </c>
+      <c r="B3001" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3001" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3001" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3001" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3001" t="n">
+        <v>105</v>
+      </c>
+      <c r="G3001" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3001" t="n">
+        <v>56</v>
+      </c>
+      <c r="I3001" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3002">
+      <c r="A3002" s="1" t="n">
+        <v>44011.7977922222</v>
+      </c>
+      <c r="B3002" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3002" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3002" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3002" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3002" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3002" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3002" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3002" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3003">
+      <c r="A3003" s="1" t="n">
+        <v>44012.0072278472</v>
+      </c>
+      <c r="B3003" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3003" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3003" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3003" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3003" t="n">
+        <v>39</v>
+      </c>
+      <c r="G3003" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3003" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3003" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3004">
+      <c r="A3004" s="1" t="n">
+        <v>44012.3363301736</v>
+      </c>
+      <c r="B3004" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3004" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3004" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3004" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3004" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3004" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3004" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3004" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3005">
+      <c r="A3005" s="1" t="n">
+        <v>44012.3596428588</v>
+      </c>
+      <c r="B3005" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3005" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3005" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3005" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3005" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3005" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3005" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3005" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3006">
+      <c r="A3006" s="1" t="n">
+        <v>44012.3819791319</v>
+      </c>
+      <c r="B3006" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3006" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3006" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3006" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3006" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3006" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3006" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3006" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3007">
+      <c r="A3007" s="1" t="n">
+        <v>44012.3773989583</v>
+      </c>
+      <c r="B3007" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3007" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3007" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3007" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3007" t="n">
+        <v>11</v>
+      </c>
+      <c r="G3007" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3007" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3007" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3008">
+      <c r="A3008" s="1" t="n">
+        <v>44012.3902007639</v>
+      </c>
+      <c r="B3008" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3008" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3008" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3008" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3008" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3008" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3008" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3008" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3009">
+      <c r="A3009" s="1" t="n">
+        <v>44012.3961870255</v>
+      </c>
+      <c r="B3009" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3009" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3009" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3009" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3009" t="n">
+        <v>34</v>
+      </c>
+      <c r="G3009" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3009" t="n">
+        <v>7</v>
+      </c>
+      <c r="I3009" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3010">
+      <c r="A3010" s="1" t="n">
+        <v>44012.4096757176</v>
+      </c>
+      <c r="B3010" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3010" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3010" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3010" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3010" t="n">
+        <v>105</v>
+      </c>
+      <c r="G3010" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3010" t="n">
+        <v>56</v>
+      </c>
+      <c r="I3010" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3011">
+      <c r="A3011" s="1" t="n">
+        <v>44012.4105323032</v>
+      </c>
+      <c r="B3011" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3011" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3011" t="n">
+        <v>127</v>
+      </c>
+      <c r="E3011" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3011" t="n">
+        <v>106</v>
+      </c>
+      <c r="G3011" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3011" t="n">
+        <v>48</v>
+      </c>
+      <c r="I3011" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3012">
+      <c r="A3012" s="1" t="n">
+        <v>44012.411678287</v>
+      </c>
+      <c r="B3012" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3012" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3012" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3012" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3012" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3012" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3012" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3012" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3013">
+      <c r="A3013" s="1" t="n">
+        <v>44012.4123125231</v>
+      </c>
+      <c r="B3013" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3013" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3013" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3013" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3013" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3013" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3013" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3013" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3014">
+      <c r="A3014" s="1" t="n">
+        <v>44012.4318107407</v>
+      </c>
+      <c r="B3014" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3014" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3014" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3014" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3014" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3014" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3014" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3014" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3015">
+      <c r="A3015" s="1" t="n">
+        <v>44012.4379437037</v>
+      </c>
+      <c r="B3015" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3015" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3015" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3015" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3015" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3015" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3015" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3015" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3016">
+      <c r="A3016" s="1" t="n">
+        <v>44012.4379699074</v>
+      </c>
+      <c r="B3016" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3016" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3016" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3016" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3016" t="n">
+        <v>45</v>
+      </c>
+      <c r="G3016" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3016" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3016" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3017">
+      <c r="A3017" s="1" t="n">
+        <v>44012.4379755208</v>
+      </c>
+      <c r="B3017" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3017" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3017" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3017" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3017" t="n">
+        <v>44</v>
+      </c>
+      <c r="G3017" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3017" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3017" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3018">
+      <c r="A3018" s="1" t="n">
+        <v>44012.4380284491</v>
+      </c>
+      <c r="B3018" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3018" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3018" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3018" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3018" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3018" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3018" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3018" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3019">
+      <c r="A3019" s="1" t="n">
+        <v>44012.4380760764</v>
+      </c>
+      <c r="B3019" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3019" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3019" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3019" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3019" t="n">
+        <v>47</v>
+      </c>
+      <c r="G3019" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3019" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3019" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3020">
+      <c r="A3020" s="1" t="n">
+        <v>44012.4380823264</v>
+      </c>
+      <c r="B3020" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3020" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3020" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3020" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3020" t="n">
+        <v>52</v>
+      </c>
+      <c r="G3020" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3020" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3020" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3021">
+      <c r="A3021" s="1" t="n">
+        <v>44012.4381356713</v>
+      </c>
+      <c r="B3021" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3021" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3021" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3021" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3021" t="n">
+        <v>48</v>
+      </c>
+      <c r="G3021" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3021" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3021" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Funcionante mas não consegui incluir os suspeitos.
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -451,6 +451,15 @@
   <si>
     <t xml:space="preserve">taivrg@gmail.com</t>
   </si>
+  <si>
+    <t xml:space="preserve">tvargas@ghc.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laurenghion@santacasa.org.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vdaudt@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -88394,6 +88403,642 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3022">
+      <c r="A3022" s="1" t="n">
+        <v>44012.4430840972</v>
+      </c>
+      <c r="B3022" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3022" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3022" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3022" t="n">
+        <v>14</v>
+      </c>
+      <c r="F3022" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3022" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3022" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3022" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3023">
+      <c r="A3023" s="1" t="n">
+        <v>44012.4432810532</v>
+      </c>
+      <c r="B3023" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3023" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3023" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3023" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3023" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3023" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3023" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3023" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3024">
+      <c r="A3024" s="1" t="n">
+        <v>44012.4437168403</v>
+      </c>
+      <c r="B3024" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3024" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3024" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3024" t="n">
+        <v>14</v>
+      </c>
+      <c r="F3024" t="n">
+        <v>37</v>
+      </c>
+      <c r="G3024" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3024" t="n">
+        <v>13</v>
+      </c>
+      <c r="I3024" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3025">
+      <c r="A3025" s="1" t="n">
+        <v>44012.4444546528</v>
+      </c>
+      <c r="B3025" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3025" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3025" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3025" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3025" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3025" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3025" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3025" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3026">
+      <c r="A3026" s="1" t="n">
+        <v>44012.4506066898</v>
+      </c>
+      <c r="B3026" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3026" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3026" t="n">
+        <v>56</v>
+      </c>
+      <c r="E3026" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3026" t="n">
+        <v>55</v>
+      </c>
+      <c r="G3026" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3026" t="n">
+        <v>16</v>
+      </c>
+      <c r="I3026" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3027">
+      <c r="A3027" s="1" t="n">
+        <v>44012.4592675694</v>
+      </c>
+      <c r="B3027" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3027" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3027" t="n">
+        <v>75</v>
+      </c>
+      <c r="E3027" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3027" t="n">
+        <v>71</v>
+      </c>
+      <c r="G3027" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3027" t="n">
+        <v>31</v>
+      </c>
+      <c r="I3027" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3028">
+      <c r="A3028" s="1" t="n">
+        <v>44012.4629340972</v>
+      </c>
+      <c r="B3028" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3028" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3028" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3028" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3028" t="n">
+        <v>33</v>
+      </c>
+      <c r="G3028" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3028" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3028" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3029">
+      <c r="A3029" s="1" t="n">
+        <v>44012.4634143171</v>
+      </c>
+      <c r="B3029" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3029" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3029" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3029" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3029" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3029" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3029" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3029" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3030">
+      <c r="A3030" s="1" t="n">
+        <v>44012.4638987384</v>
+      </c>
+      <c r="B3030" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3030" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3030" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3030" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3030" t="n">
+        <v>67</v>
+      </c>
+      <c r="G3030" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3030" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3030" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3031">
+      <c r="A3031" s="1" t="n">
+        <v>44012.4880545023</v>
+      </c>
+      <c r="B3031" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3031" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3031" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3031" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3031" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3031" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3031" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3031" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3032">
+      <c r="A3032" s="1" t="n">
+        <v>44012.4978171643</v>
+      </c>
+      <c r="B3032" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3032" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3032" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3032" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3032" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3032" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3032" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3032" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3033">
+      <c r="A3033" s="1" t="n">
+        <v>44012.5939550232</v>
+      </c>
+      <c r="B3033" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3033" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3033" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3033" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3033" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3033" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3033" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3033" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3034">
+      <c r="A3034" s="1" t="n">
+        <v>44012.6140535532</v>
+      </c>
+      <c r="B3034" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3034" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3034" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3034" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3034" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3034" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3034" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3034" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3035">
+      <c r="A3035" s="1" t="n">
+        <v>44012.7018351852</v>
+      </c>
+      <c r="B3035" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3035" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3035" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3035" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3035" t="n">
+        <v>39</v>
+      </c>
+      <c r="G3035" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3035" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3035" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3036">
+      <c r="A3036" s="1" t="n">
+        <v>44012.7163709722</v>
+      </c>
+      <c r="B3036" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3036" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3036" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3036" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3036" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3036" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3036" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3036" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3037">
+      <c r="A3037" s="1" t="n">
+        <v>44012.7601441667</v>
+      </c>
+      <c r="B3037" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3037" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3037" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3037" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3037" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3037" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3037" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3037" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3038">
+      <c r="A3038" s="1" t="n">
+        <v>44012.7608082176</v>
+      </c>
+      <c r="B3038" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3038"/>
+      <c r="D3038" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3038" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3038" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3038" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3038" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3038" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3039">
+      <c r="A3039" s="1" t="n">
+        <v>44012.8023355324</v>
+      </c>
+      <c r="B3039" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3039" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3039" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3039" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3039" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3039" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3039" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3039" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3040">
+      <c r="A3040" s="1" t="n">
+        <v>44012.8511676157</v>
+      </c>
+      <c r="B3040" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3040" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3040" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3040" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3040" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3040" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3040" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3040" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3041">
+      <c r="A3041" s="1" t="n">
+        <v>44012.8523852083</v>
+      </c>
+      <c r="B3041" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3041" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3041" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3041" t="n">
+        <v>14</v>
+      </c>
+      <c r="F3041" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3041" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3041" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3041" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3042">
+      <c r="A3042" s="1" t="n">
+        <v>44012.8946015394</v>
+      </c>
+      <c r="B3042" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3042" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3042" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3042" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3042" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3042" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3042" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3042" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3043">
+      <c r="A3043" s="1" t="n">
+        <v>44012.9705118287</v>
+      </c>
+      <c r="B3043" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3043" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3043" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3043" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3043" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3043" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3043" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3043" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Versão funcional, antes da tentativa de inclusão da distribuição dos suspeitos
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -460,6 +460,9 @@
   <si>
     <t xml:space="preserve">vdaudt@gmail.com</t>
   </si>
+  <si>
+    <t xml:space="preserve">adriano.silva@pucrs.br</t>
+  </si>
 </sst>
 </file>
 
@@ -89039,6 +89042,1742 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3044">
+      <c r="A3044" s="1" t="n">
+        <v>44013.3365863773</v>
+      </c>
+      <c r="B3044" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3044" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3044" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3044" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3044" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3044" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3044" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3044" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3045">
+      <c r="A3045" s="1" t="n">
+        <v>44013.3709671181</v>
+      </c>
+      <c r="B3045" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3045" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3045" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3045" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3045" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3045" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3045" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3045" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3046">
+      <c r="A3046" s="1" t="n">
+        <v>44013.3850510995</v>
+      </c>
+      <c r="B3046" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3046" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3046" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3046" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3046" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3046" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3046" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3046" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3047">
+      <c r="A3047" s="1" t="n">
+        <v>44013.3851965509</v>
+      </c>
+      <c r="B3047" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3047" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3047" t="n">
+        <v>132</v>
+      </c>
+      <c r="E3047" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3047" t="n">
+        <v>97</v>
+      </c>
+      <c r="G3047" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3047" t="n">
+        <v>51</v>
+      </c>
+      <c r="I3047" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3048">
+      <c r="A3048" s="1" t="n">
+        <v>44013.3910863657</v>
+      </c>
+      <c r="B3048" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3048" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3048" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3048" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3048" t="n">
+        <v>11</v>
+      </c>
+      <c r="G3048" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3048" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3048" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3049">
+      <c r="A3049" s="1" t="n">
+        <v>44013.3912461111</v>
+      </c>
+      <c r="B3049" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3049" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3049" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3049" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3049" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3049" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3049" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3049" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3050">
+      <c r="A3050" s="1" t="n">
+        <v>44013.4140563773</v>
+      </c>
+      <c r="B3050" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3050" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3050" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3050" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3050" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3050" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3050" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3050" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3051">
+      <c r="A3051" s="1" t="n">
+        <v>44013.4205393403</v>
+      </c>
+      <c r="B3051" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3051" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3051" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3051" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3051" t="n">
+        <v>58</v>
+      </c>
+      <c r="G3051" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3051" t="n">
+        <v>17</v>
+      </c>
+      <c r="I3051" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3052">
+      <c r="A3052" s="1" t="n">
+        <v>44013.4216951852</v>
+      </c>
+      <c r="B3052" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3052" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3052" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3052" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3052" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3052" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3052" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3052" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3053">
+      <c r="A3053" s="1" t="n">
+        <v>44013.4444204167</v>
+      </c>
+      <c r="B3053" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3053" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3053" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3053" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3053" t="n">
+        <v>37</v>
+      </c>
+      <c r="G3053" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3053" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3053" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3054">
+      <c r="A3054" s="1" t="n">
+        <v>44013.4470134375</v>
+      </c>
+      <c r="B3054" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3054" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3054" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3054" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3054" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3054" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3054" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3054" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3055">
+      <c r="A3055" s="1" t="n">
+        <v>44013.4490095949</v>
+      </c>
+      <c r="B3055" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3055" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3055" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3055" t="n">
+        <v>40</v>
+      </c>
+      <c r="F3055" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3055" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3055" t="n">
+        <v>7</v>
+      </c>
+      <c r="I3055" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3056">
+      <c r="A3056" s="1" t="n">
+        <v>44013.4501532986</v>
+      </c>
+      <c r="B3056" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3056" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3056" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3056" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3056" t="n">
+        <v>27</v>
+      </c>
+      <c r="G3056" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3056" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3056" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3057">
+      <c r="A3057" s="1" t="n">
+        <v>44013.4551684491</v>
+      </c>
+      <c r="B3057" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3057" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3057" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3057" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3057" t="n">
+        <v>45</v>
+      </c>
+      <c r="G3057" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3057" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3057" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3058">
+      <c r="A3058" s="1" t="n">
+        <v>44013.4663389583</v>
+      </c>
+      <c r="B3058" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3058" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3058" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3058" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3058" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3058" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3058" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3058" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3059">
+      <c r="A3059" s="1" t="n">
+        <v>44013.4677818866</v>
+      </c>
+      <c r="B3059" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3059" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3059" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3059" t="n">
+        <v>14</v>
+      </c>
+      <c r="F3059" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3059" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3059" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3059" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3060">
+      <c r="A3060" s="1" t="n">
+        <v>44013.4812394097</v>
+      </c>
+      <c r="B3060" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3060" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3060" t="n">
+        <v>75</v>
+      </c>
+      <c r="E3060" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3060" t="n">
+        <v>71</v>
+      </c>
+      <c r="G3060" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3060" t="n">
+        <v>33</v>
+      </c>
+      <c r="I3060" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3061">
+      <c r="A3061" s="1" t="n">
+        <v>44013.482673287</v>
+      </c>
+      <c r="B3061" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3061"/>
+      <c r="D3061" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3061" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3061" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3061" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3061" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3061" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3062">
+      <c r="A3062" s="1" t="n">
+        <v>44013.4831484722</v>
+      </c>
+      <c r="B3062" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3062"/>
+      <c r="D3062" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3062" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3062" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3062" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3062" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3062" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3063">
+      <c r="A3063" s="1" t="n">
+        <v>44013.4981880787</v>
+      </c>
+      <c r="B3063" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3063" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3063" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3063" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3063" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3063" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3063" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3063" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3064">
+      <c r="A3064" s="1" t="n">
+        <v>44013.5298350347</v>
+      </c>
+      <c r="B3064" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3064" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3064" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3064" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3064" t="n">
+        <v>74</v>
+      </c>
+      <c r="G3064" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3064" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3064" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3065">
+      <c r="A3065" s="1" t="n">
+        <v>44013.5307931018</v>
+      </c>
+      <c r="B3065" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3065" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3065" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3065" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3065" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3065" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3065" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3065" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3066">
+      <c r="A3066" s="1" t="n">
+        <v>44013.5809336806</v>
+      </c>
+      <c r="B3066" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3066" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3066" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3066" t="n">
+        <v>14</v>
+      </c>
+      <c r="F3066" t="n">
+        <v>42</v>
+      </c>
+      <c r="G3066" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3066" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3066" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3067">
+      <c r="A3067" s="1" t="n">
+        <v>44013.591476088</v>
+      </c>
+      <c r="B3067" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3067" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3067" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3067" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3067" t="n">
+        <v>38</v>
+      </c>
+      <c r="G3067" t="n">
+        <v>15</v>
+      </c>
+      <c r="H3067" t="n">
+        <v>12</v>
+      </c>
+      <c r="I3067" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3068">
+      <c r="A3068" s="1" t="n">
+        <v>44013.6173689352</v>
+      </c>
+      <c r="B3068" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3068" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3068" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3068" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3068" t="n">
+        <v>13</v>
+      </c>
+      <c r="G3068" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3068" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3068" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3069">
+      <c r="A3069" s="1" t="n">
+        <v>44013.6898032176</v>
+      </c>
+      <c r="B3069" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3069" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3069" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3069" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3069" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3069" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3069" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3069" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3070">
+      <c r="A3070" s="1" t="n">
+        <v>44013.6974801852</v>
+      </c>
+      <c r="B3070" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3070" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3070" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3070" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3070" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3070" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3070" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3070" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3071">
+      <c r="A3071" s="1" t="n">
+        <v>44013.7422103588</v>
+      </c>
+      <c r="B3071" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3071" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3071" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3071" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3071" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3071" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3071" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3071" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3072">
+      <c r="A3072" s="1" t="n">
+        <v>44013.7602301273</v>
+      </c>
+      <c r="B3072" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3072" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3072" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3072" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3072" t="n">
+        <v>29</v>
+      </c>
+      <c r="G3072" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3072" t="n">
+        <v>13</v>
+      </c>
+      <c r="I3072" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3073">
+      <c r="A3073" s="1" t="n">
+        <v>44013.7783539815</v>
+      </c>
+      <c r="B3073" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3073" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3073" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3073" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3073" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3073" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3073" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3073" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3074">
+      <c r="A3074" s="1" t="n">
+        <v>44013.7811551157</v>
+      </c>
+      <c r="B3074" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3074" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3074" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3074" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3074" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3074" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3074" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3074" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3075">
+      <c r="A3075" s="1" t="n">
+        <v>44013.7844894444</v>
+      </c>
+      <c r="B3075" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3075" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3075" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3075" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3075" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3075" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3075" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3075" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3076">
+      <c r="A3076" s="1" t="n">
+        <v>44013.8028936805</v>
+      </c>
+      <c r="B3076" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3076" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3076" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3076" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3076" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3076" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3076" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3076" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3077">
+      <c r="A3077" s="1" t="n">
+        <v>44013.854121331</v>
+      </c>
+      <c r="B3077" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3077" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3077" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3077" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3077" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3077" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3077" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3077" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3078">
+      <c r="A3078" s="1" t="n">
+        <v>44014.0047878125</v>
+      </c>
+      <c r="B3078" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3078" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3078" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3078" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3078" t="n">
+        <v>27</v>
+      </c>
+      <c r="G3078" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3078" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3078" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3079">
+      <c r="A3079" s="1" t="n">
+        <v>44014.317369132</v>
+      </c>
+      <c r="B3079" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3079" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3079" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3079" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3079" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3079" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3079" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3079" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3080">
+      <c r="A3080" s="1" t="n">
+        <v>44014.3265892361</v>
+      </c>
+      <c r="B3080" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3080" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3080" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3080" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3080" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3080" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3080" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3080" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3081">
+      <c r="A3081" s="1" t="n">
+        <v>44014.3380972685</v>
+      </c>
+      <c r="B3081" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3081" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3081" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3081" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3081" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3081" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3081" t="n">
+        <v>13</v>
+      </c>
+      <c r="I3081" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3082">
+      <c r="A3082" s="1" t="n">
+        <v>44014.3481868634</v>
+      </c>
+      <c r="B3082" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3082" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3082" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3082" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3082" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3082" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3082" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3082" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3083">
+      <c r="A3083" s="1" t="n">
+        <v>44014.3774703125</v>
+      </c>
+      <c r="B3083" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3083" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3083" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3083" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3083" t="n">
+        <v>11</v>
+      </c>
+      <c r="G3083" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3083" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3083" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3084">
+      <c r="A3084" s="1" t="n">
+        <v>44014.3941892708</v>
+      </c>
+      <c r="B3084" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3084" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3084" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3084" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3084" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3084" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3084" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3084" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3085">
+      <c r="A3085" s="1" t="n">
+        <v>44014.4007195486</v>
+      </c>
+      <c r="B3085" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3085" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3085" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3085" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3085" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3085" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3085" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3085" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3086">
+      <c r="A3086" s="1" t="n">
+        <v>44014.4031798843</v>
+      </c>
+      <c r="B3086" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3086" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3086" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3086" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3086" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3086" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3086" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3086" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3087">
+      <c r="A3087" s="1" t="n">
+        <v>44014.4053894792</v>
+      </c>
+      <c r="B3087" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3087" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3087" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3087" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3087" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3087" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3087" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3087" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3088">
+      <c r="A3088" s="1" t="n">
+        <v>44014.4071360301</v>
+      </c>
+      <c r="B3088" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3088" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3088" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3088" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3088" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3088" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3088" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3088" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3089">
+      <c r="A3089" s="1" t="n">
+        <v>44014.4133712153</v>
+      </c>
+      <c r="B3089" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3089" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3089" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3089" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3089" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3089" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3089" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3089" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3090">
+      <c r="A3090" s="1" t="n">
+        <v>44014.4212634722</v>
+      </c>
+      <c r="B3090" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3090" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3090" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3090" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3090" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3090" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3090" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3090" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3091">
+      <c r="A3091" s="1" t="n">
+        <v>44014.4250166088</v>
+      </c>
+      <c r="B3091" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3091" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3091" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3091" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3091" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3091" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3091" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3091" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3092">
+      <c r="A3092" s="1" t="n">
+        <v>44014.4254803472</v>
+      </c>
+      <c r="B3092" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3092" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3092" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3092" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3092" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3092" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3092" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3092" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3093">
+      <c r="A3093" s="1" t="n">
+        <v>44014.4355262037</v>
+      </c>
+      <c r="B3093" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3093" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3093" t="n">
+        <v>132</v>
+      </c>
+      <c r="E3093" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3093" t="n">
+        <v>112</v>
+      </c>
+      <c r="G3093" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3093" t="n">
+        <v>55</v>
+      </c>
+      <c r="I3093" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3094">
+      <c r="A3094" s="1" t="n">
+        <v>44014.4372751736</v>
+      </c>
+      <c r="B3094" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3094" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3094" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3094" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3094" t="n">
+        <v>53</v>
+      </c>
+      <c r="G3094" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3094" t="n">
+        <v>17</v>
+      </c>
+      <c r="I3094" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3095">
+      <c r="A3095" s="1" t="n">
+        <v>44014.4487356713</v>
+      </c>
+      <c r="B3095" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3095" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3095" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3095" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3095" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3095" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3095" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3095" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3096">
+      <c r="A3096" s="1" t="n">
+        <v>44014.4566375694</v>
+      </c>
+      <c r="B3096" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3096" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3096" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3096" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3096" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3096" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3096" t="n">
+        <v>17</v>
+      </c>
+      <c r="I3096" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3097">
+      <c r="A3097" s="1" t="n">
+        <v>44014.4718456597</v>
+      </c>
+      <c r="B3097" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3097" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3097" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3097" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3097" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3097" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3097" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3097" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3098">
+      <c r="A3098" s="1" t="n">
+        <v>44014.4765016088</v>
+      </c>
+      <c r="B3098" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3098" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3098" t="n">
+        <v>75</v>
+      </c>
+      <c r="E3098" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3098" t="n">
+        <v>70</v>
+      </c>
+      <c r="G3098" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3098" t="n">
+        <v>34</v>
+      </c>
+      <c r="I3098" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3099">
+      <c r="A3099" s="1" t="n">
+        <v>44014.4779293403</v>
+      </c>
+      <c r="B3099" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3099" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3099" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3099" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3099" t="n">
+        <v>45</v>
+      </c>
+      <c r="G3099" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3099" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3099" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3100">
+      <c r="A3100" s="1" t="n">
+        <v>44014.4794104167</v>
+      </c>
+      <c r="B3100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3100" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3100" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3100" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3100" t="n">
+        <v>45</v>
+      </c>
+      <c r="G3100" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3100" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3100" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3101">
+      <c r="A3101" s="1" t="n">
+        <v>44014.4971597454</v>
+      </c>
+      <c r="B3101" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3101" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3101" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3101" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3101" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3101" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3101" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3101" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3102">
+      <c r="A3102" s="1" t="n">
+        <v>44014.4990697454</v>
+      </c>
+      <c r="B3102" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3102" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3102" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3102" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3102" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3102" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3102" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3103">
+      <c r="A3103" s="1" t="n">
+        <v>44014.4991938773</v>
+      </c>
+      <c r="B3103" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3103" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3103" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3103" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3103" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3103" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3103" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Ajustes dos rótulos do gráfico
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -90778,6 +90778,1326 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3104">
+      <c r="A3104" s="1" t="n">
+        <v>44014.5250114699</v>
+      </c>
+      <c r="B3104" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3104"/>
+      <c r="D3104" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3104" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3104" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3104" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3105">
+      <c r="A3105" s="1" t="n">
+        <v>44014.5388523495</v>
+      </c>
+      <c r="B3105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3105" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3105" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3105" t="n">
+        <v>83</v>
+      </c>
+      <c r="G3105" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3105" t="n">
+        <v>17</v>
+      </c>
+      <c r="I3105" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3106">
+      <c r="A3106" s="1" t="n">
+        <v>44014.5397035648</v>
+      </c>
+      <c r="B3106" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3106" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3106" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3106" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3106" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3106" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3106" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3107">
+      <c r="A3107" s="1" t="n">
+        <v>44014.5698651505</v>
+      </c>
+      <c r="B3107" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3107"/>
+      <c r="D3107" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3107" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3107" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3107" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3108">
+      <c r="A3108" s="1" t="n">
+        <v>44014.570281956</v>
+      </c>
+      <c r="B3108" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3108"/>
+      <c r="D3108" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3108" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3108" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3108" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3109">
+      <c r="A3109" s="1" t="n">
+        <v>44014.6248022685</v>
+      </c>
+      <c r="B3109" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3109"/>
+      <c r="D3109" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3109" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3109" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3109" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3109" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3110">
+      <c r="A3110" s="1" t="n">
+        <v>44014.6524191088</v>
+      </c>
+      <c r="B3110" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3110" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3110" t="n">
+        <v>21</v>
+      </c>
+      <c r="E3110" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3110" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3110" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3110" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3110" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3111">
+      <c r="A3111" s="1" t="n">
+        <v>44014.706859537</v>
+      </c>
+      <c r="B3111" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3111" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3111" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3111" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3111" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3111" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3111" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3111" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3112">
+      <c r="A3112" s="1" t="n">
+        <v>44014.7244074537</v>
+      </c>
+      <c r="B3112" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3112"/>
+      <c r="D3112" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3112" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3112" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3112" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3112" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3112" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3113">
+      <c r="A3113" s="1" t="n">
+        <v>44014.7928018981</v>
+      </c>
+      <c r="B3113" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3113" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3113" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3113" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3113" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3113" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3113" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3114">
+      <c r="A3114" s="1" t="n">
+        <v>44014.8617557292</v>
+      </c>
+      <c r="B3114" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3114" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3114" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3114" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3114" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3114" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3114" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3115">
+      <c r="A3115" s="1" t="n">
+        <v>44014.9533616319</v>
+      </c>
+      <c r="B3115" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3115" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3115" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3115" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3115" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3115" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3115" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3116">
+      <c r="A3116" s="1" t="n">
+        <v>44015.3276058681</v>
+      </c>
+      <c r="B3116" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3116" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3116" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3116" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3116" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3116" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3116" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3117">
+      <c r="A3117" s="1" t="n">
+        <v>44015.342424375</v>
+      </c>
+      <c r="B3117" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3117" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3117" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3117" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3117" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3117" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3117" t="n">
+        <v>16</v>
+      </c>
+      <c r="I3117" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3118">
+      <c r="A3118" s="1" t="n">
+        <v>44015.3505016551</v>
+      </c>
+      <c r="B3118" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3118" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3118" t="n">
+        <v>22</v>
+      </c>
+      <c r="E3118" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3118" t="n">
+        <v>15</v>
+      </c>
+      <c r="G3118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3118" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3118" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3119">
+      <c r="A3119" s="1" t="n">
+        <v>44015.3656844097</v>
+      </c>
+      <c r="B3119" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3119" t="n">
+        <v>22</v>
+      </c>
+      <c r="E3119" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3119" t="n">
+        <v>15</v>
+      </c>
+      <c r="G3119" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3119" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3119" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3120">
+      <c r="A3120" s="1" t="n">
+        <v>44015.3703084028</v>
+      </c>
+      <c r="B3120" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3120" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3120" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3120" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3120" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3120" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3120" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3121">
+      <c r="A3121" s="1" t="n">
+        <v>44015.372710081</v>
+      </c>
+      <c r="B3121" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3121" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3121" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3121" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3121" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3121" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3122">
+      <c r="A3122" s="1" t="n">
+        <v>44015.3741301736</v>
+      </c>
+      <c r="B3122" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3122" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3122" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3122" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3122" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3122" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3122" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3123">
+      <c r="A3123" s="1" t="n">
+        <v>44015.3792889583</v>
+      </c>
+      <c r="B3123" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3123" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3123" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3123" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3123" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3123" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3124">
+      <c r="A3124" s="1" t="n">
+        <v>44015.3860435648</v>
+      </c>
+      <c r="B3124" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3124" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3124" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3124" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3124" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3124" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3124" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3124" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3125">
+      <c r="A3125" s="1" t="n">
+        <v>44015.3910035532</v>
+      </c>
+      <c r="B3125" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3125" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3125" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3125" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3125" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3125" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3125" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3125" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3126">
+      <c r="A3126" s="1" t="n">
+        <v>44015.4011600694</v>
+      </c>
+      <c r="B3126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3126" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3126" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3126" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3126" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3126" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3126" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3126" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3127">
+      <c r="A3127" s="1" t="n">
+        <v>44015.4012519676</v>
+      </c>
+      <c r="B3127" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3127" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3127" t="n">
+        <v>75</v>
+      </c>
+      <c r="E3127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3127" t="n">
+        <v>69</v>
+      </c>
+      <c r="G3127" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3127" t="n">
+        <v>35</v>
+      </c>
+      <c r="I3127" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3128">
+      <c r="A3128" s="1" t="n">
+        <v>44015.4130154514</v>
+      </c>
+      <c r="B3128" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3128" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3128" t="n">
+        <v>132</v>
+      </c>
+      <c r="E3128" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3128" t="n">
+        <v>112</v>
+      </c>
+      <c r="G3128" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3128" t="n">
+        <v>55</v>
+      </c>
+      <c r="I3128" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3129">
+      <c r="A3129" s="1" t="n">
+        <v>44015.4158879745</v>
+      </c>
+      <c r="B3129" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3129" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3129" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3129" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3129" t="n">
+        <v>112</v>
+      </c>
+      <c r="G3129" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3129" t="n">
+        <v>66</v>
+      </c>
+      <c r="I3129" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3130">
+      <c r="A3130" s="1" t="n">
+        <v>44015.4176060648</v>
+      </c>
+      <c r="B3130" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3130" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3130" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3130" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3130" t="n">
+        <v>112</v>
+      </c>
+      <c r="G3130" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3130" t="n">
+        <v>60</v>
+      </c>
+      <c r="I3130" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3131">
+      <c r="A3131" s="1" t="n">
+        <v>44015.4209084838</v>
+      </c>
+      <c r="B3131" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3131" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3131" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3131" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3131" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3131" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3131" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3132">
+      <c r="A3132" s="1" t="n">
+        <v>44015.4230039699</v>
+      </c>
+      <c r="B3132" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3132" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3132" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3132" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3132" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3132" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3132" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3132" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3133">
+      <c r="A3133" s="1" t="n">
+        <v>44015.4263795949</v>
+      </c>
+      <c r="B3133" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3133" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3133" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3133" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3133" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3133" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3133" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3134">
+      <c r="A3134" s="1" t="n">
+        <v>44015.4336391667</v>
+      </c>
+      <c r="B3134" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3134" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3134" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3134" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3134" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3134" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3134" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3134" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3135">
+      <c r="A3135" s="1" t="n">
+        <v>44015.4534153241</v>
+      </c>
+      <c r="B3135" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3135" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3135" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3135" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3135" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3135" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3135" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3136">
+      <c r="A3136" s="1" t="n">
+        <v>44015.4536779051</v>
+      </c>
+      <c r="B3136" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3136" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3136" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3136" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3136" t="n">
+        <v>49</v>
+      </c>
+      <c r="G3136" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3136" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3136" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3137">
+      <c r="A3137" s="1" t="n">
+        <v>44015.4543685301</v>
+      </c>
+      <c r="B3137" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3137" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3137" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3137" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3137" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3137" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3137" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3138">
+      <c r="A3138" s="1" t="n">
+        <v>44015.4674844907</v>
+      </c>
+      <c r="B3138" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3138" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3138" t="n">
+        <v>62</v>
+      </c>
+      <c r="E3138" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3138" t="n">
+        <v>62</v>
+      </c>
+      <c r="G3138" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3138" t="n">
+        <v>18</v>
+      </c>
+      <c r="I3138" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3139">
+      <c r="A3139" s="1" t="n">
+        <v>44015.4742865625</v>
+      </c>
+      <c r="B3139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3139" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3139" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3139" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3139" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3139" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3139" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3139" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3140">
+      <c r="A3140" s="1" t="n">
+        <v>44015.4752991088</v>
+      </c>
+      <c r="B3140" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3140" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3140" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3140" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3140" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3140" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3140" t="n">
+        <v>17</v>
+      </c>
+      <c r="I3140" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3141">
+      <c r="A3141" s="1" t="n">
+        <v>44015.4875017593</v>
+      </c>
+      <c r="B3141" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3141"/>
+      <c r="D3141" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3141" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3141" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3141" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3142">
+      <c r="A3142" s="1" t="n">
+        <v>44015.4882807755</v>
+      </c>
+      <c r="B3142" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3142"/>
+      <c r="D3142" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3142" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3142" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3142" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3142" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3143">
+      <c r="A3143" s="1" t="n">
+        <v>44015.4904919444</v>
+      </c>
+      <c r="B3143" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3143" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3143" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3143" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3143" t="n">
+        <v>84</v>
+      </c>
+      <c r="G3143" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3143" t="n">
+        <v>22</v>
+      </c>
+      <c r="I3143" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3144">
+      <c r="A3144" s="1" t="n">
+        <v>44015.4907811574</v>
+      </c>
+      <c r="B3144" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3144" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3144" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3144" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3144" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3144" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3144" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3145">
+      <c r="A3145" s="1" t="n">
+        <v>44015.5254097454</v>
+      </c>
+      <c r="B3145" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3145" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3145" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3145" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3145" t="n">
+        <v>11</v>
+      </c>
+      <c r="G3145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3145" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3145" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3146">
+      <c r="A3146" s="1" t="n">
+        <v>44015.6072373264</v>
+      </c>
+      <c r="B3146" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3146" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3146" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3146" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3146" t="n">
+        <v>30</v>
+      </c>
+      <c r="G3146" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3146" t="n">
+        <v>6</v>
+      </c>
+      <c r="I3146" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3147">
+      <c r="A3147" s="1" t="n">
+        <v>44015.6479794907</v>
+      </c>
+      <c r="B3147" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3147" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3147" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3147" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3147" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3147" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3147" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3147" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3148">
+      <c r="A3148" s="1" t="n">
+        <v>44015.6874309607</v>
+      </c>
+      <c r="B3148" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3148" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3148" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3148" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3148" t="n">
+        <v>45</v>
+      </c>
+      <c r="G3148" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3148" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3148" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3149">
+      <c r="A3149" s="1" t="n">
+        <v>44015.7881525347</v>
+      </c>
+      <c r="B3149" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3149" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3149" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3149" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3149" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3149" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3149" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3149" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Tentativas de trazer o carregamento das UTIs pra dentro do app
</commit_message>
<xml_diff>
--- a/Corona/uti.xlsx
+++ b/Corona/uti.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -463,6 +463,12 @@
   <si>
     <t xml:space="preserve">adriano.silva@pucrs.br</t>
   </si>
+  <si>
+    <t xml:space="preserve">roberta.marco@pucrs.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vdaudt@gmail.con</t>
+  </si>
 </sst>
 </file>
 
@@ -92098,6 +92104,1825 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3150">
+      <c r="A3150" s="1" t="n">
+        <v>44016.3555861343</v>
+      </c>
+      <c r="B3150" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3150" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3150" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3150" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3150" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3150" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3150" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3150" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3151">
+      <c r="A3151" s="1" t="n">
+        <v>44016.3717638657</v>
+      </c>
+      <c r="B3151" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3151" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3151" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3151" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3151" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3151" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3151" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3152">
+      <c r="A3152" s="1" t="n">
+        <v>44016.3816875694</v>
+      </c>
+      <c r="B3152" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3152" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3152" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3152" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3152" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3152" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3152" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3153">
+      <c r="A3153" s="1" t="n">
+        <v>44016.3845214699</v>
+      </c>
+      <c r="B3153" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3153"/>
+      <c r="D3153" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3153" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3153" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3153" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3153" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3153" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3154">
+      <c r="A3154" s="1" t="n">
+        <v>44016.3849317824</v>
+      </c>
+      <c r="B3154" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3154"/>
+      <c r="D3154" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3154" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3154" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3154" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3154" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3154" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3155">
+      <c r="A3155" s="1" t="n">
+        <v>44016.3850471991</v>
+      </c>
+      <c r="B3155" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3155" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3155" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3155" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3155" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3155" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3155" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3155" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3156">
+      <c r="A3156" s="1" t="n">
+        <v>44016.3930456481</v>
+      </c>
+      <c r="B3156" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3156" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3156" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3156" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3156" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3156" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3156" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3156" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3157">
+      <c r="A3157" s="1" t="n">
+        <v>44016.3970703935</v>
+      </c>
+      <c r="B3157" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3157" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3157" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3157" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3157" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3157" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3157" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3157" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3158">
+      <c r="A3158" s="1" t="n">
+        <v>44016.4000319676</v>
+      </c>
+      <c r="B3158" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3158" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3158" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3158" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3158" t="n">
+        <v>33</v>
+      </c>
+      <c r="G3158" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3158" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3158" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3159">
+      <c r="A3159" s="1" t="n">
+        <v>44016.4272566667</v>
+      </c>
+      <c r="B3159" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3159" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3159" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3159" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3159" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3159" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3159" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3159" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3160">
+      <c r="A3160" s="1" t="n">
+        <v>44016.4285894213</v>
+      </c>
+      <c r="B3160" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3160" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3160" t="n">
+        <v>55</v>
+      </c>
+      <c r="E3160" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3160" t="n">
+        <v>49</v>
+      </c>
+      <c r="G3160" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3160" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3160" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3161">
+      <c r="A3161" s="1" t="n">
+        <v>44016.4377929514</v>
+      </c>
+      <c r="B3161" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3161" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3161" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3161" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3161" t="n">
+        <v>38</v>
+      </c>
+      <c r="G3161" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3161" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3161" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3162">
+      <c r="A3162" s="1" t="n">
+        <v>44016.4448094329</v>
+      </c>
+      <c r="B3162" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3162" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3162" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3162" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3162" t="n">
+        <v>112</v>
+      </c>
+      <c r="G3162" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3162" t="n">
+        <v>60</v>
+      </c>
+      <c r="I3162" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3163">
+      <c r="A3163" s="1" t="n">
+        <v>44016.4460376389</v>
+      </c>
+      <c r="B3163" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3163" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3163" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3163" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3163" t="n">
+        <v>113</v>
+      </c>
+      <c r="G3163" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3163" t="n">
+        <v>66</v>
+      </c>
+      <c r="I3163" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3164">
+      <c r="A3164" s="1" t="n">
+        <v>44016.4486981944</v>
+      </c>
+      <c r="B3164" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3164" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3164" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3164" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3164" t="n">
+        <v>113</v>
+      </c>
+      <c r="G3164" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3164" t="n">
+        <v>61</v>
+      </c>
+      <c r="I3164" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3165">
+      <c r="A3165" s="1" t="n">
+        <v>44016.4516996991</v>
+      </c>
+      <c r="B3165" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3165" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3165" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3165" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3165" t="n">
+        <v>75</v>
+      </c>
+      <c r="G3165" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3165" t="n">
+        <v>18</v>
+      </c>
+      <c r="I3165" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3166">
+      <c r="A3166" s="1" t="n">
+        <v>44016.4543020833</v>
+      </c>
+      <c r="B3166" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3166" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3166" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3166" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3166" t="n">
+        <v>29</v>
+      </c>
+      <c r="G3166" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3166" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3166" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3167">
+      <c r="A3167" s="1" t="n">
+        <v>44016.466665625</v>
+      </c>
+      <c r="B3167" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3167" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3167" t="n">
+        <v>62</v>
+      </c>
+      <c r="E3167" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3167" t="n">
+        <v>55</v>
+      </c>
+      <c r="G3167" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3167" t="n">
+        <v>19</v>
+      </c>
+      <c r="I3167" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3168">
+      <c r="A3168" s="1" t="n">
+        <v>44016.4689364005</v>
+      </c>
+      <c r="B3168" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3168" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3168" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3168" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3168" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3168" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3168" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3168" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3169">
+      <c r="A3169" s="1" t="n">
+        <v>44016.4697260301</v>
+      </c>
+      <c r="B3169" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3169" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3169" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3169" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3169" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3169" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3169" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3169" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3170">
+      <c r="A3170" s="1" t="n">
+        <v>44016.5402731944</v>
+      </c>
+      <c r="B3170" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3170" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3170" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3170" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3170" t="n">
+        <v>49</v>
+      </c>
+      <c r="G3170" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3170" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3170" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3171">
+      <c r="A3171" s="1" t="n">
+        <v>44016.5484452894</v>
+      </c>
+      <c r="B3171" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3171" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3171" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3171" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3171" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3171" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3171" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3172">
+      <c r="A3172" s="1" t="n">
+        <v>44016.567486875</v>
+      </c>
+      <c r="B3172" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3172" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3172" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3172" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3172" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3172" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3172" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3172" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3173">
+      <c r="A3173" s="1" t="n">
+        <v>44016.5715396643</v>
+      </c>
+      <c r="B3173" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3173" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3173" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3173" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3173" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3173" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3173" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3173" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3174">
+      <c r="A3174" s="1" t="n">
+        <v>44016.6113953704</v>
+      </c>
+      <c r="B3174" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3174" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3174" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3174" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3174" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3174" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3174" t="n">
+        <v>19</v>
+      </c>
+      <c r="I3174" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3175">
+      <c r="A3175" s="1" t="n">
+        <v>44016.633203044</v>
+      </c>
+      <c r="B3175" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3175" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3175" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3175" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3175" t="n">
+        <v>36</v>
+      </c>
+      <c r="G3175" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3175" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3175" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3176">
+      <c r="A3176" s="1" t="n">
+        <v>44016.6400973032</v>
+      </c>
+      <c r="B3176" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3176" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3176" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3176" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3176" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3176" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3176" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3176" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3177">
+      <c r="A3177" s="1" t="n">
+        <v>44016.6448118634</v>
+      </c>
+      <c r="B3177" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3177" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3177" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3177" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3177" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3177" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3177" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3177" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3178">
+      <c r="A3178" s="1" t="n">
+        <v>44016.7053432986</v>
+      </c>
+      <c r="B3178" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3178" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3178" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3178" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3178" t="n">
+        <v>113</v>
+      </c>
+      <c r="G3178" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3178" t="n">
+        <v>61</v>
+      </c>
+      <c r="I3178" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3179">
+      <c r="A3179" s="1" t="n">
+        <v>44016.7231890741</v>
+      </c>
+      <c r="B3179" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3179" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3179" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3179" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3179" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3179" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3179" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3179" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3180">
+      <c r="A3180" s="1" t="n">
+        <v>44016.7283023611</v>
+      </c>
+      <c r="B3180" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3180" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3180" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3180" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3180" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3180" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3180" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3180" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3181">
+      <c r="A3181" s="1" t="n">
+        <v>44016.7503557523</v>
+      </c>
+      <c r="B3181" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3181" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3181" t="n">
+        <v>75</v>
+      </c>
+      <c r="E3181" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3181" t="n">
+        <v>68</v>
+      </c>
+      <c r="G3181" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3181" t="n">
+        <v>32</v>
+      </c>
+      <c r="I3181" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3182">
+      <c r="A3182" s="1" t="n">
+        <v>44016.9693852431</v>
+      </c>
+      <c r="B3182" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3182" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3182" t="n">
+        <v>75</v>
+      </c>
+      <c r="E3182" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3182" t="n">
+        <v>62</v>
+      </c>
+      <c r="G3182" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3182" t="n">
+        <v>27</v>
+      </c>
+      <c r="I3182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3183">
+      <c r="A3183" s="1" t="n">
+        <v>44017.0619679398</v>
+      </c>
+      <c r="B3183" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3183" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3183" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3183" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3183" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3183" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3183" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3183" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3184">
+      <c r="A3184" s="1" t="n">
+        <v>44017.0640566319</v>
+      </c>
+      <c r="B3184" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3184" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3184" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3184" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3184" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3184" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3184" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3184" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3185">
+      <c r="A3185" s="1" t="n">
+        <v>44017.3185566782</v>
+      </c>
+      <c r="B3185" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3185" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3185" t="n">
+        <v>40</v>
+      </c>
+      <c r="E3185" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3185" t="n">
+        <v>33</v>
+      </c>
+      <c r="G3185" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3185" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3185" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3186">
+      <c r="A3186" s="1" t="n">
+        <v>44017.3376250694</v>
+      </c>
+      <c r="B3186" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3186" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3186" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3186" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3186" t="n">
+        <v>34</v>
+      </c>
+      <c r="G3186" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3186" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3186" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3187">
+      <c r="A3187" s="1" t="n">
+        <v>44017.3630550463</v>
+      </c>
+      <c r="B3187" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3187" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3187" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3187" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3187" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3187" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3187" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3187" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3188">
+      <c r="A3188" s="1" t="n">
+        <v>44017.3946934722</v>
+      </c>
+      <c r="B3188" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3188" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3188" t="n">
+        <v>13</v>
+      </c>
+      <c r="E3188" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3188" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3188" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3188" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3188" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3189">
+      <c r="A3189" s="1" t="n">
+        <v>44017.4191157639</v>
+      </c>
+      <c r="B3189" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3189" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3189" t="n">
+        <v>62</v>
+      </c>
+      <c r="E3189" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3189" t="n">
+        <v>56</v>
+      </c>
+      <c r="G3189" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3189" t="n">
+        <v>19</v>
+      </c>
+      <c r="I3189" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3190">
+      <c r="A3190" s="1" t="n">
+        <v>44017.4303852778</v>
+      </c>
+      <c r="B3190" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3190" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3190" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3190" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3190" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3190" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3190" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3190" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3191">
+      <c r="A3191" s="1" t="n">
+        <v>44017.4385067708</v>
+      </c>
+      <c r="B3191" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3191" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3191" t="n">
+        <v>48</v>
+      </c>
+      <c r="E3191" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3191" t="n">
+        <v>38</v>
+      </c>
+      <c r="G3191" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3191" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3191" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3192">
+      <c r="A3192" s="1" t="n">
+        <v>44017.441231956</v>
+      </c>
+      <c r="B3192" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3192" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3192" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3192" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3192" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3192" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3192" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3192" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3193">
+      <c r="A3193" s="1" t="n">
+        <v>44017.4427331481</v>
+      </c>
+      <c r="B3193" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3193" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3193" t="n">
+        <v>38</v>
+      </c>
+      <c r="E3193" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3193" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3193" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3193" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3193" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3194">
+      <c r="A3194" s="1" t="n">
+        <v>44017.4519614583</v>
+      </c>
+      <c r="B3194" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3194" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3194" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3194" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3194" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3194" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3194" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3194" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3195">
+      <c r="A3195" s="1" t="n">
+        <v>44017.4549542824</v>
+      </c>
+      <c r="B3195" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3195" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3195" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3195" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3195" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3195" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3195" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3195" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3196">
+      <c r="A3196" s="1" t="n">
+        <v>44017.4586382292</v>
+      </c>
+      <c r="B3196" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3196" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3196" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3196" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3196" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3196" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3196" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3196" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3197">
+      <c r="A3197" s="1" t="n">
+        <v>44017.4658776968</v>
+      </c>
+      <c r="B3197" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3197" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3197" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3197" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3197" t="n">
+        <v>19</v>
+      </c>
+      <c r="G3197" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3197" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3197" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3198">
+      <c r="A3198" s="1" t="n">
+        <v>44017.472314294</v>
+      </c>
+      <c r="B3198" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3198" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3198" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3198" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3198" t="n">
+        <v>35</v>
+      </c>
+      <c r="G3198" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3198" t="n">
+        <v>16</v>
+      </c>
+      <c r="I3198" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3199">
+      <c r="A3199" s="1" t="n">
+        <v>44017.4768285648</v>
+      </c>
+      <c r="B3199" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3199" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3199" t="n">
+        <v>101</v>
+      </c>
+      <c r="E3199" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3199" t="n">
+        <v>75</v>
+      </c>
+      <c r="G3199" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3199" t="n">
+        <v>18</v>
+      </c>
+      <c r="I3199" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3200">
+      <c r="A3200" s="1" t="n">
+        <v>44017.4775991898</v>
+      </c>
+      <c r="B3200" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3200" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3200" t="n">
+        <v>37</v>
+      </c>
+      <c r="E3200" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3200" t="n">
+        <v>27</v>
+      </c>
+      <c r="G3200" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3200" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3200" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3201">
+      <c r="A3201" s="1" t="n">
+        <v>44017.4823460301</v>
+      </c>
+      <c r="B3201" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3201" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3201" t="n">
+        <v>135</v>
+      </c>
+      <c r="E3201" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3201" t="n">
+        <v>113</v>
+      </c>
+      <c r="G3201" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3201" t="n">
+        <v>61</v>
+      </c>
+      <c r="I3201" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3202">
+      <c r="A3202" s="1" t="n">
+        <v>44017.4832879861</v>
+      </c>
+      <c r="B3202" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3202" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3202" t="n">
+        <v>137</v>
+      </c>
+      <c r="E3202" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3202" t="n">
+        <v>117</v>
+      </c>
+      <c r="G3202" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3202" t="n">
+        <v>60</v>
+      </c>
+      <c r="I3202" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3203">
+      <c r="A3203" s="1" t="n">
+        <v>44017.4892809838</v>
+      </c>
+      <c r="B3203" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3203"/>
+      <c r="D3203" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3203" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3203" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3203" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3203" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3203" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3204">
+      <c r="A3204" s="1" t="n">
+        <v>44017.4900394097</v>
+      </c>
+      <c r="B3204" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3204"/>
+      <c r="D3204" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3204" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3204" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3204" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3204" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3204" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3205">
+      <c r="A3205" s="1" t="n">
+        <v>44017.4946845139</v>
+      </c>
+      <c r="B3205" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3205" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3205" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3205" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3205" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3205" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3205" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3205" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3206">
+      <c r="A3206" s="1" t="n">
+        <v>44017.5159593634</v>
+      </c>
+      <c r="B3206" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3206" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3206" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3206" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3206" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3206" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3206" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3206" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3207">
+      <c r="A3207" s="1" t="n">
+        <v>44017.5358270718</v>
+      </c>
+      <c r="B3207" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3207" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3207" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3207" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3207" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3207" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3207" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3207" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3208">
+      <c r="A3208" s="1" t="n">
+        <v>44017.5443161227</v>
+      </c>
+      <c r="B3208" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3208" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3208" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3208" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3208" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3208" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3208" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3208" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3209">
+      <c r="A3209" s="1" t="n">
+        <v>44017.5464031134</v>
+      </c>
+      <c r="B3209" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3209" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3209" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3209" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3209" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3209" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3209" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3209" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3210">
+      <c r="A3210" s="1" t="n">
+        <v>44017.5554215625</v>
+      </c>
+      <c r="B3210" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3210" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3210" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3210" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3210" t="n">
+        <v>19</v>
+      </c>
+      <c r="G3210" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3210" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3210" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3211">
+      <c r="A3211" s="1" t="n">
+        <v>44017.5751993518</v>
+      </c>
+      <c r="B3211" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3211" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3211" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3211" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3211" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3211" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3211" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3211" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3212">
+      <c r="A3212" s="1" t="n">
+        <v>44017.5836446759</v>
+      </c>
+      <c r="B3212" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3212" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3212" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3212" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3212" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3212" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3212" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3212" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>